<commit_message>
USD,EUR,AUD,JPY market refresh at 07 aug 2014
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD_Market.xlsx
@@ -2483,70 +2483,70 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 18:00:06</v>
         <stp/>
-        <stp>{E5B2F945-91E2-4CB2-8408-8B1D9E8826B0}</stp>
+        <stp>{2D4C3CC7-464E-4148-A89C-DE660E02AB7B}</stp>
+        <tr r="O4" s="18"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:59:27</v>
+        <stp/>
+        <stp>{29DD0DE5-16AD-4B48-84E1-0F534444688D}</stp>
+        <tr r="Q5" s="64"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:59:27</v>
+        <stp/>
+        <stp>{8CA828FA-C977-44F0-AA79-128C07B4ACFC}</stp>
+        <tr r="O2" s="17"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:59:27</v>
+        <stp/>
+        <stp>{B93B1D57-0BAB-4994-A9B8-D0BDAB07616B}</stp>
         <tr r="P4" s="26"/>
       </tp>
       <tp t="s">
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
         <stp/>
-        <stp>{33F71036-CA46-4418-8124-AD5DAB2BA34B}</stp>
+        <stp>{9EC21750-2124-4906-A30C-BDA4A7B436C0}</stp>
+        <tr r="P4" s="25"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:59:27</v>
+        <stp/>
+        <stp>{A84219F8-11A9-4903-B445-5C6C3E099C42}</stp>
+        <tr r="O4" s="65"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:59:27</v>
+        <stp/>
+        <stp>{AAE7DFF3-4320-4331-91F7-E4CDAA56CF57}</stp>
+        <tr r="M4" s="22"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:59:27</v>
+        <stp/>
+        <stp>{51212936-057E-4425-97A7-AB711E07D6A4}</stp>
+        <tr r="P4" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:59:27</v>
+        <stp/>
+        <stp>{FCA40E4F-D48C-483A-9D94-301F3054E529}</stp>
         <tr r="J4" s="15"/>
       </tp>
       <tp t="s">
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
         <stp/>
-        <stp>{920619D3-BC71-4C6F-8221-1E9CF09DE67C}</stp>
-        <tr r="O4" s="65"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 11:09:33</v>
-        <stp/>
-        <stp>{F848B6B6-CB32-470D-904D-BA32DBD094AF}</stp>
-        <tr r="Q5" s="64"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 11:09:55</v>
-        <stp/>
-        <stp>{DB0E7866-A1F7-4630-9AE3-8B647F7519B5}</stp>
-        <tr r="O4" s="18"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 11:09:33</v>
-        <stp/>
-        <stp>{1B3F1E3E-E783-40A0-93E8-6D62A4871FC7}</stp>
-        <tr r="O2" s="17"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 11:09:33</v>
-        <stp/>
-        <stp>{8DC426FA-0A24-4002-BA64-CF904C8C472A}</stp>
-        <tr r="P4" s="25"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 11:09:33</v>
-        <stp/>
-        <stp>{F2C9149B-4311-45B2-AC7E-5CD60AE5CBB9}</stp>
-        <tr r="P4" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 11:09:33</v>
-        <stp/>
-        <stp>{5D993C85-41E5-4FEE-BA08-D892368A50C0}</stp>
+        <stp>{FD2B0DFD-BB4C-4DD2-9D12-58A8A951B40A}</stp>
         <tr r="P4" s="11"/>
       </tp>
       <tp t="s">
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
         <stp/>
-        <stp>{7BDEEC00-7D7D-4D05-898D-74836301E66E}</stp>
+        <stp>{09237A72-05AE-44C9-AA72-A39318EB7771}</stp>
         <tr r="N4" s="16"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 11:09:33</v>
-        <stp/>
-        <stp>{432CD8AE-3EDE-4239-8408-5CFE55409E78}</stp>
-        <tr r="M4" s="22"/>
       </tp>
     </main>
   </volType>
@@ -2914,7 +2914,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="351">
-        <v>41850.464548611111</v>
+        <v>41858.749212962961</v>
       </c>
       <c r="E5" s="9"/>
       <c r="G5" s="126"/>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="D7" s="353">
         <f>_xll.ohTrigger(Deposits!R3,FRA!X3,Futures3M!Z3,FuturesHWConvAdj!Q3,Swap3M!Z3,Swap6M!Z3,BasisSwap1M3M!X3,BasisSwap3M6M!X3,OIS!W3)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7" s="9"/>
       <c r="G7" s="126"/>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="D8" s="353">
         <f>_xll.ohTrigger(BBSW!W6:W12)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E8" s="9"/>
       <c r="G8" s="126"/>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="I10" s="358">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>41850</v>
+        <v>41858</v>
       </c>
       <c r="J10" s="204"/>
     </row>
@@ -3201,7 +3201,7 @@
         <v>163</v>
       </c>
       <c r="D22" s="367">
-        <v>41809.384120370371</v>
+        <v>41858.750034722223</v>
       </c>
       <c r="E22" s="9"/>
       <c r="G22" s="8"/>
@@ -3351,7 +3351,7 @@
       <c r="P3" s="51"/>
       <c r="Q3" s="123">
         <f>_xll.ohTrigger(Q5:Q9)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R3" s="9"/>
       <c r="S3" s="3"/>
@@ -3766,7 +3766,7 @@
       <c r="O4" s="79"/>
       <c r="P4" s="330" t="str">
         <f>_xll.RData(P5:P42,Q4:T4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="Q4" s="143" t="s">
         <v>130</v>
@@ -3923,10 +3923,10 @@
         <v>AUDQM3AB1Y=ICAA</v>
       </c>
       <c r="Q6" s="101">
-        <v>2.6025</v>
+        <v>2.56</v>
       </c>
       <c r="R6" s="101">
-        <v>2.6525000000000003</v>
+        <v>2.6100000000000003</v>
       </c>
       <c r="S6" s="101">
         <v>0</v>
@@ -3936,19 +3936,19 @@
       </c>
       <c r="U6" s="104">
         <f>_xll.qlMidSafe($Q6,$R6)</f>
-        <v>2.6275000000000004</v>
+        <v>2.585</v>
       </c>
       <c r="V6" s="102"/>
       <c r="W6" s="103">
-        <v>2.6749999999999998</v>
+        <v>2.585</v>
       </c>
       <c r="X6" s="102"/>
       <c r="Y6" s="154">
-        <v>2.6275000000000004</v>
+        <v>2.585</v>
       </c>
       <c r="Z6" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F6,Y6/100,Trigger)</f>
-        <v>-4.9999999999997963E-5</v>
+        <v>-4.2500000000000523E-4</v>
       </c>
       <c r="AA6" s="90"/>
       <c r="AB6" s="3"/>
@@ -4231,10 +4231,10 @@
         <v>AUDQM3AB2Y=ICAA</v>
       </c>
       <c r="Q10" s="101">
-        <v>2.6975000000000002</v>
+        <v>2.66</v>
       </c>
       <c r="R10" s="101">
-        <v>2.7575000000000003</v>
+        <v>2.72</v>
       </c>
       <c r="S10" s="101">
         <v>0</v>
@@ -4244,19 +4244,19 @@
       </c>
       <c r="U10" s="104">
         <f>_xll.qlMidSafe($Q10,$R10)</f>
-        <v>2.7275</v>
+        <v>2.6900000000000004</v>
       </c>
       <c r="V10" s="102"/>
       <c r="W10" s="103">
-        <v>2.7850000000000001</v>
+        <v>2.6900000000000004</v>
       </c>
       <c r="X10" s="102"/>
       <c r="Y10" s="154">
-        <v>2.7275</v>
+        <v>2.6900000000000004</v>
       </c>
       <c r="Z10" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F10,Y10/100,Trigger)</f>
-        <v>-1.2500000000000011E-4</v>
+        <v>-3.7499999999999686E-4</v>
       </c>
       <c r="AA10" s="90"/>
       <c r="AB10" s="3"/>
@@ -4308,10 +4308,10 @@
         <v>AUDQM3AB3Y=ICAA</v>
       </c>
       <c r="Q11" s="101">
-        <v>2.8425000000000002</v>
+        <v>2.8225000000000002</v>
       </c>
       <c r="R11" s="101">
-        <v>2.9025000000000003</v>
+        <v>2.8825000000000003</v>
       </c>
       <c r="S11" s="101">
         <v>0</v>
@@ -4321,19 +4321,19 @@
       </c>
       <c r="U11" s="104">
         <f>_xll.qlMidSafe($Q11,$R11)</f>
-        <v>2.8725000000000005</v>
+        <v>2.8525</v>
       </c>
       <c r="V11" s="102"/>
       <c r="W11" s="103">
-        <v>2.9349999999999996</v>
+        <v>2.8525</v>
       </c>
       <c r="X11" s="102"/>
       <c r="Y11" s="154">
-        <v>2.8725000000000005</v>
+        <v>2.8525</v>
       </c>
       <c r="Z11" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F11,Y11/100,Trigger)</f>
-        <v>-1.4999999999999736E-4</v>
+        <v>-2.0000000000000226E-4</v>
       </c>
       <c r="AA11" s="90"/>
       <c r="AB11" s="3"/>
@@ -6946,7 +6946,7 @@
       <c r="O4" s="79"/>
       <c r="P4" s="98" t="str">
         <f>_xll.RData(P5:P42,Q4:T4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="Q4" s="143" t="s">
         <v>130</v>
@@ -7565,10 +7565,10 @@
         <v>AUDSM6AB4Y=ICAA</v>
       </c>
       <c r="Q12" s="101">
-        <v>3.0725000000000002</v>
+        <v>3.0675000000000003</v>
       </c>
       <c r="R12" s="101">
-        <v>3.1325000000000003</v>
+        <v>3.1274999999999999</v>
       </c>
       <c r="S12" s="101">
         <v>0</v>
@@ -7578,7 +7578,7 @@
       </c>
       <c r="U12" s="104">
         <f>_xll.qlMidEquivalent($Q12,$R12,$S12,$T12)</f>
-        <v>3.1025</v>
+        <v>3.0975000000000001</v>
       </c>
       <c r="V12" s="102"/>
       <c r="W12" s="103">
@@ -7586,11 +7586,11 @@
       </c>
       <c r="X12" s="102"/>
       <c r="Y12" s="154">
-        <v>3.1025</v>
+        <v>3.0975000000000001</v>
       </c>
       <c r="Z12" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F12,Y12/100,Trigger)</f>
-        <v>-2.5000000000000369E-4</v>
+        <v>-4.9999999999997963E-5</v>
       </c>
       <c r="AA12" s="90"/>
       <c r="AB12" s="3"/>
@@ -7642,10 +7642,10 @@
         <v>AUDSM6AB5Y=ICAA</v>
       </c>
       <c r="Q13" s="101">
-        <v>3.2175000000000002</v>
+        <v>3.2250000000000001</v>
       </c>
       <c r="R13" s="101">
-        <v>3.2775000000000003</v>
+        <v>3.2850000000000001</v>
       </c>
       <c r="S13" s="101">
         <v>0</v>
@@ -7655,7 +7655,7 @@
       </c>
       <c r="U13" s="104">
         <f>_xll.qlMidEquivalent($Q13,$R13,$S13,$T13)</f>
-        <v>3.2475000000000005</v>
+        <v>3.2549999999999999</v>
       </c>
       <c r="V13" s="102"/>
       <c r="W13" s="103">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="X13" s="102"/>
       <c r="Y13" s="154">
-        <v>3.2475000000000005</v>
+        <v>3.2549999999999999</v>
       </c>
       <c r="Z13" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F13,Y13/100,Trigger)</f>
-        <v>-4.2499999999999483E-4</v>
+        <v>7.499999999999174E-5</v>
       </c>
       <c r="AA13" s="90"/>
       <c r="AB13" s="3"/>
@@ -7719,10 +7719,10 @@
         <v>AUDSM6AB6Y=ICAA</v>
       </c>
       <c r="Q14" s="101">
-        <v>3.3650000000000002</v>
+        <v>3.375</v>
       </c>
       <c r="R14" s="101">
-        <v>3.4250000000000003</v>
+        <v>3.4350000000000001</v>
       </c>
       <c r="S14" s="101">
         <v>0</v>
@@ -7732,7 +7732,7 @@
       </c>
       <c r="U14" s="104">
         <f>_xll.qlMidEquivalent($Q14,$R14,$S14,$T14)</f>
-        <v>3.3950000000000005</v>
+        <v>3.4050000000000002</v>
       </c>
       <c r="V14" s="102"/>
       <c r="W14" s="103">
@@ -7740,11 +7740,11 @@
       </c>
       <c r="X14" s="102"/>
       <c r="Y14" s="154">
-        <v>3.3950000000000005</v>
+        <v>3.4050000000000002</v>
       </c>
       <c r="Z14" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F14,Y14/100,Trigger)</f>
-        <v>-5.4999999999999494E-4</v>
+        <v>9.9999999999995925E-5</v>
       </c>
       <c r="AA14" s="90"/>
       <c r="AB14" s="3"/>
@@ -7796,10 +7796,10 @@
         <v>AUDSM6AB7Y=ICAA</v>
       </c>
       <c r="Q15" s="101">
-        <v>3.4950000000000001</v>
+        <v>3.5075000000000003</v>
       </c>
       <c r="R15" s="101">
-        <v>3.5550000000000002</v>
+        <v>3.5675000000000003</v>
       </c>
       <c r="S15" s="101">
         <v>0</v>
@@ -7809,7 +7809,7 @@
       </c>
       <c r="U15" s="104">
         <f>_xll.qlMidEquivalent($Q15,$R15,$S15,$T15)</f>
-        <v>3.5250000000000004</v>
+        <v>3.5375000000000005</v>
       </c>
       <c r="V15" s="102"/>
       <c r="W15" s="103">
@@ -7817,11 +7817,11 @@
       </c>
       <c r="X15" s="102"/>
       <c r="Y15" s="154">
-        <v>3.5250000000000004</v>
+        <v>3.5375000000000005</v>
       </c>
       <c r="Z15" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F15,Y15/100,Trigger)</f>
-        <v>-6.9999999999999923E-4</v>
+        <v>1.2500000000000011E-4</v>
       </c>
       <c r="AA15" s="90"/>
       <c r="AB15" s="3"/>
@@ -7873,10 +7873,10 @@
         <v>AUDSM6AB8Y=ICAA</v>
       </c>
       <c r="Q16" s="101">
-        <v>3.605</v>
+        <v>3.6225000000000001</v>
       </c>
       <c r="R16" s="101">
-        <v>3.665</v>
+        <v>3.6825000000000001</v>
       </c>
       <c r="S16" s="101">
         <v>0</v>
@@ -7886,7 +7886,7 @@
       </c>
       <c r="U16" s="104">
         <f>_xll.qlMidEquivalent($Q16,$R16,$S16,$T16)</f>
-        <v>3.6349999999999998</v>
+        <v>3.6524999999999999</v>
       </c>
       <c r="V16" s="102"/>
       <c r="W16" s="103">
@@ -7894,11 +7894,11 @@
       </c>
       <c r="X16" s="102"/>
       <c r="Y16" s="154">
-        <v>3.6349999999999998</v>
+        <v>3.6524999999999999</v>
       </c>
       <c r="Z16" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F16,Y16/100,Trigger)</f>
-        <v>-8.2499999999999934E-4</v>
+        <v>1.7500000000000154E-4</v>
       </c>
       <c r="AA16" s="90"/>
       <c r="AB16" s="3"/>
@@ -7950,10 +7950,10 @@
         <v>AUDSM6AB9Y=ICAA</v>
       </c>
       <c r="Q17" s="101">
-        <v>3.7</v>
+        <v>3.7175000000000002</v>
       </c>
       <c r="R17" s="101">
-        <v>3.7600000000000002</v>
+        <v>3.7775000000000003</v>
       </c>
       <c r="S17" s="101">
         <v>0</v>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="U17" s="104">
         <f>_xll.qlMidEquivalent($Q17,$R17,$S17,$T17)</f>
-        <v>3.7300000000000004</v>
+        <v>3.7475000000000005</v>
       </c>
       <c r="V17" s="102"/>
       <c r="W17" s="103">
@@ -7971,11 +7971,11 @@
       </c>
       <c r="X17" s="102"/>
       <c r="Y17" s="154">
-        <v>3.7300000000000004</v>
+        <v>3.7475000000000005</v>
       </c>
       <c r="Z17" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F17,Y17/100,Trigger)</f>
-        <v>-9.2499999999998833E-4</v>
+        <v>1.7500000000000154E-4</v>
       </c>
       <c r="AA17" s="90"/>
       <c r="AB17" s="3"/>
@@ -8027,10 +8027,10 @@
         <v>AUDSM6AB10Y=ICAA</v>
       </c>
       <c r="Q18" s="101">
-        <v>3.7875000000000001</v>
+        <v>3.8050000000000002</v>
       </c>
       <c r="R18" s="101">
-        <v>3.8475000000000001</v>
+        <v>3.8650000000000002</v>
       </c>
       <c r="S18" s="101">
         <v>0</v>
@@ -8040,7 +8040,7 @@
       </c>
       <c r="U18" s="104">
         <f>_xll.qlMidEquivalent($Q18,$R18,$S18,$T18)</f>
-        <v>3.8174999999999999</v>
+        <v>3.835</v>
       </c>
       <c r="V18" s="102"/>
       <c r="W18" s="103">
@@ -8048,11 +8048,11 @@
       </c>
       <c r="X18" s="102"/>
       <c r="Y18" s="154">
-        <v>3.8174999999999999</v>
+        <v>3.835</v>
       </c>
       <c r="Z18" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F18,Y18/100,Trigger)</f>
-        <v>-9.749999999999967E-4</v>
+        <v>1.7500000000000154E-4</v>
       </c>
       <c r="AA18" s="90"/>
       <c r="AB18" s="3"/>
@@ -8181,10 +8181,10 @@
         <v>AUDSM6AB12Y=ICAA</v>
       </c>
       <c r="Q20" s="101">
-        <v>3.9350000000000001</v>
+        <v>3.9525000000000001</v>
       </c>
       <c r="R20" s="101">
-        <v>3.9950000000000001</v>
+        <v>4.0125000000000002</v>
       </c>
       <c r="S20" s="101">
         <v>0</v>
@@ -8194,7 +8194,7 @@
       </c>
       <c r="U20" s="104">
         <f>_xll.qlMidEquivalent($Q20,$R20,$S20,$T20)</f>
-        <v>3.9649999999999999</v>
+        <v>3.9824999999999999</v>
       </c>
       <c r="V20" s="102"/>
       <c r="W20" s="103">
@@ -8202,11 +8202,11 @@
       </c>
       <c r="X20" s="102"/>
       <c r="Y20" s="154">
-        <v>3.9649999999999999</v>
+        <v>3.9824999999999999</v>
       </c>
       <c r="Z20" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F20,Y20/100,Trigger)</f>
-        <v>-1.1000000000000038E-3</v>
+        <v>1.7500000000000154E-4</v>
       </c>
       <c r="AA20" s="90"/>
       <c r="AB20" s="3"/>
@@ -8412,10 +8412,10 @@
         <v>AUDSM6AB15Y=ICAA</v>
       </c>
       <c r="Q23" s="101">
-        <v>4.07</v>
+        <v>4.0875000000000004</v>
       </c>
       <c r="R23" s="101">
-        <v>4.1500000000000004</v>
+        <v>4.1675000000000004</v>
       </c>
       <c r="S23" s="101">
         <v>0</v>
@@ -8425,7 +8425,7 @@
       </c>
       <c r="U23" s="104">
         <f>_xll.qlMidEquivalent($Q23,$R23,$S23,$T23)</f>
-        <v>4.1100000000000003</v>
+        <v>4.1275000000000004</v>
       </c>
       <c r="V23" s="102"/>
       <c r="W23" s="103">
@@ -8433,11 +8433,11 @@
       </c>
       <c r="X23" s="102"/>
       <c r="Y23" s="154">
-        <v>4.1100000000000003</v>
+        <v>4.1275000000000004</v>
       </c>
       <c r="Z23" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F23,Y23/100,Trigger)</f>
-        <v>-1.1249999999999941E-3</v>
+        <v>1.7500000000000154E-4</v>
       </c>
       <c r="AA23" s="90"/>
       <c r="AB23" s="3"/>
@@ -8797,10 +8797,10 @@
         <v>AUDSM6AB20Y=ICAA</v>
       </c>
       <c r="Q28" s="101">
-        <v>4.2050000000000001</v>
+        <v>4.2200000000000006</v>
       </c>
       <c r="R28" s="101">
-        <v>4.2850000000000001</v>
+        <v>4.3</v>
       </c>
       <c r="S28" s="101">
         <v>0</v>
@@ -8810,7 +8810,7 @@
       </c>
       <c r="U28" s="104">
         <f>_xll.qlMidEquivalent($Q28,$R28,$S28,$T28)</f>
-        <v>4.2450000000000001</v>
+        <v>4.26</v>
       </c>
       <c r="V28" s="102"/>
       <c r="W28" s="103">
@@ -8818,11 +8818,11 @@
       </c>
       <c r="X28" s="102"/>
       <c r="Y28" s="154">
-        <v>4.2450000000000001</v>
+        <v>4.26</v>
       </c>
       <c r="Z28" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F28,Y28/100,Trigger)</f>
-        <v>-9.7500000000000364E-4</v>
+        <v>1.4999999999999736E-4</v>
       </c>
       <c r="AA28" s="90"/>
       <c r="AB28" s="3"/>
@@ -9182,10 +9182,10 @@
         <v>AUDSM6AB25Y=ICAA</v>
       </c>
       <c r="Q33" s="101">
-        <v>4.2525000000000004</v>
+        <v>4.2700000000000005</v>
       </c>
       <c r="R33" s="101">
-        <v>4.3325000000000005</v>
+        <v>4.3500000000000005</v>
       </c>
       <c r="S33" s="101">
         <v>0</v>
@@ -9195,7 +9195,7 @@
       </c>
       <c r="U33" s="104">
         <f>_xll.qlMidEquivalent($Q33,$R33,$S33,$T33)</f>
-        <v>4.2925000000000004</v>
+        <v>4.3100000000000005</v>
       </c>
       <c r="V33" s="102"/>
       <c r="W33" s="103">
@@ -9203,11 +9203,11 @@
       </c>
       <c r="X33" s="102"/>
       <c r="Y33" s="154">
-        <v>4.2925000000000004</v>
+        <v>4.3100000000000005</v>
       </c>
       <c r="Z33" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F33,Y33/100,Trigger)</f>
-        <v>-9.4999999999999946E-4</v>
+        <v>1.7500000000000154E-4</v>
       </c>
       <c r="AA33" s="90"/>
       <c r="AB33" s="3"/>
@@ -9567,10 +9567,10 @@
         <v>AUDSM6AB30Y=ICAA</v>
       </c>
       <c r="Q38" s="101">
-        <v>4.2725</v>
+        <v>4.29</v>
       </c>
       <c r="R38" s="101">
-        <v>4.3525</v>
+        <v>4.37</v>
       </c>
       <c r="S38" s="101">
         <v>0</v>
@@ -9580,7 +9580,7 @@
       </c>
       <c r="U38" s="104">
         <f>_xll.qlMidEquivalent($Q38,$R38,$S38,$T38)</f>
-        <v>4.3125</v>
+        <v>4.33</v>
       </c>
       <c r="V38" s="102"/>
       <c r="W38" s="103">
@@ -9588,11 +9588,11 @@
       </c>
       <c r="X38" s="102"/>
       <c r="Y38" s="154">
-        <v>4.3125</v>
+        <v>4.33</v>
       </c>
       <c r="Z38" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F38,Y38/100,Trigger)</f>
-        <v>-8.2500000000000628E-4</v>
+        <v>1.7500000000000154E-4</v>
       </c>
       <c r="AA38" s="90"/>
       <c r="AB38" s="3"/>
@@ -9721,10 +9721,10 @@
         <v>AUDSM6AB40Y=ICAA</v>
       </c>
       <c r="Q40" s="101">
-        <v>4.2324999999999999</v>
+        <v>4.25</v>
       </c>
       <c r="R40" s="101">
-        <v>4.3125</v>
+        <v>4.33</v>
       </c>
       <c r="S40" s="101">
         <v>0</v>
@@ -9734,7 +9734,7 @@
       </c>
       <c r="U40" s="104">
         <f>_xll.qlMidEquivalent($Q40,$R40,$S40,$T40)</f>
-        <v>4.2725</v>
+        <v>4.29</v>
       </c>
       <c r="V40" s="102"/>
       <c r="W40" s="103">
@@ -9742,11 +9742,11 @@
       </c>
       <c r="X40" s="102"/>
       <c r="Y40" s="154">
-        <v>4.2725</v>
+        <v>4.29</v>
       </c>
       <c r="Z40" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F40,Y40/100,Trigger)</f>
-        <v>-8.2500000000000628E-4</v>
+        <v>1.7500000000000154E-4</v>
       </c>
       <c r="AA40" s="90"/>
       <c r="AB40" s="3"/>
@@ -10102,7 +10102,7 @@
       <c r="O4" s="79"/>
       <c r="P4" s="98" t="str">
         <f>_xll.RData(P5:P42,Q4:R4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="Q4" s="143" t="s">
         <v>130</v>
@@ -10181,7 +10181,7 @@
       </c>
       <c r="T5" s="102"/>
       <c r="U5" s="199">
-        <v>4.75</v>
+        <v>4.875</v>
       </c>
       <c r="V5" s="102"/>
       <c r="W5" s="208">
@@ -10190,7 +10190,7 @@
       </c>
       <c r="X5" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F5,W5/10000,Trigger)</f>
-        <v>-3.749999999999999E-5</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="90"/>
       <c r="Z5" s="3"/>
@@ -10254,7 +10254,7 @@
       </c>
       <c r="T6" s="102"/>
       <c r="U6" s="199">
-        <v>5.5</v>
+        <v>5.25</v>
       </c>
       <c r="V6" s="102"/>
       <c r="W6" s="208">
@@ -10262,7 +10262,7 @@
       </c>
       <c r="X6" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/10000,Trigger)</f>
-        <v>-3.749999999999999E-5</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="90"/>
       <c r="Z6" s="3"/>
@@ -10532,7 +10532,7 @@
       </c>
       <c r="T10" s="102"/>
       <c r="U10" s="199">
-        <v>6.5</v>
+        <v>6.25</v>
       </c>
       <c r="V10" s="102"/>
       <c r="W10" s="208">
@@ -10540,7 +10540,7 @@
       </c>
       <c r="X10" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/10000,Trigger)</f>
-        <v>-1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="90"/>
     </row>
@@ -10588,26 +10588,26 @@
         <v>AUBR3AB3Y=ICAA</v>
       </c>
       <c r="Q11" s="200">
-        <v>5.5</v>
+        <v>5.625</v>
       </c>
       <c r="R11" s="200">
-        <v>7.5</v>
+        <v>7.625</v>
       </c>
       <c r="S11" s="191">
         <f>_xll.qlMidEquivalent(Q11,R11)</f>
-        <v>6.5</v>
+        <v>6.625</v>
       </c>
       <c r="T11" s="102"/>
       <c r="U11" s="199">
-        <v>6.75</v>
+        <v>6.625</v>
       </c>
       <c r="V11" s="102"/>
       <c r="W11" s="208">
-        <v>6.5</v>
+        <v>6.625</v>
       </c>
       <c r="X11" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/10000,Trigger)</f>
-        <v>-2.5000000000000066E-5</v>
+        <v>1.2500000000000033E-5</v>
       </c>
       <c r="Y11" s="90"/>
     </row>
@@ -10655,26 +10655,26 @@
         <v>AUBR3AB4Y=ICAA</v>
       </c>
       <c r="Q12" s="200">
-        <v>5.75</v>
+        <v>5.875</v>
       </c>
       <c r="R12" s="200">
-        <v>7.75</v>
+        <v>7.875</v>
       </c>
       <c r="S12" s="191">
         <f>_xll.qlMidEquivalent(Q12,R12)</f>
-        <v>6.75</v>
+        <v>6.875</v>
       </c>
       <c r="T12" s="102"/>
       <c r="U12" s="199">
-        <v>7.25</v>
+        <v>6.875</v>
       </c>
       <c r="V12" s="102"/>
       <c r="W12" s="208">
-        <v>6.75</v>
+        <v>6.875</v>
       </c>
       <c r="X12" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/10000,Trigger)</f>
-        <v>-2.4999999999999957E-5</v>
+        <v>1.2499999999999924E-5</v>
       </c>
       <c r="Y12" s="90"/>
     </row>
@@ -10722,26 +10722,26 @@
         <v>AUBR3AB5Y=ICAA</v>
       </c>
       <c r="Q13" s="200">
-        <v>6</v>
+        <v>6.125</v>
       </c>
       <c r="R13" s="200">
-        <v>8</v>
+        <v>8.125</v>
       </c>
       <c r="S13" s="191">
         <f>_xll.qlMidEquivalent(Q13,R13)</f>
-        <v>7</v>
+        <v>7.125</v>
       </c>
       <c r="T13" s="102"/>
       <c r="U13" s="199">
-        <v>7.5</v>
+        <v>7.125</v>
       </c>
       <c r="V13" s="102"/>
       <c r="W13" s="208">
-        <v>7</v>
+        <v>7.125</v>
       </c>
       <c r="X13" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/10000,Trigger)</f>
-        <v>-2.4999999999999957E-5</v>
+        <v>1.2500000000000033E-5</v>
       </c>
       <c r="Y13" s="90"/>
     </row>
@@ -10867,7 +10867,7 @@
       </c>
       <c r="T15" s="102"/>
       <c r="U15" s="199">
-        <v>7.625</v>
+        <v>7.5</v>
       </c>
       <c r="V15" s="102"/>
       <c r="W15" s="208">
@@ -10875,7 +10875,7 @@
       </c>
       <c r="X15" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/10000,Trigger)</f>
-        <v>-2.4999999999999957E-5</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="90"/>
     </row>
@@ -11068,7 +11068,7 @@
       </c>
       <c r="T18" s="102"/>
       <c r="U18" s="199">
-        <v>7.625</v>
+        <v>7.75</v>
       </c>
       <c r="V18" s="102"/>
       <c r="W18" s="208">
@@ -11076,7 +11076,7 @@
       </c>
       <c r="X18" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F18,W18/10000,Trigger)</f>
-        <v>-2.5000000000000066E-5</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="90"/>
       <c r="AC18"/>
@@ -11203,7 +11203,7 @@
       </c>
       <c r="T20" s="102"/>
       <c r="U20" s="199">
-        <v>7.625</v>
+        <v>7.75</v>
       </c>
       <c r="V20" s="102"/>
       <c r="W20" s="208">
@@ -11211,7 +11211,7 @@
       </c>
       <c r="X20" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F20,W20/10000,Trigger)</f>
-        <v>1.2499999999999924E-5</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="90"/>
     </row>
@@ -12893,7 +12893,7 @@
       <c r="O4" s="79"/>
       <c r="P4" s="98" t="str">
         <f>_xll.RData(P5:P42,Q4:R4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="Q4" s="143" t="s">
         <v>130</v>
@@ -12977,7 +12977,7 @@
       </c>
       <c r="T5" s="102"/>
       <c r="U5" s="199">
-        <v>3.625</v>
+        <v>3.875</v>
       </c>
       <c r="V5" s="102"/>
       <c r="W5" s="208">
@@ -12986,7 +12986,7 @@
       </c>
       <c r="X5" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F5,W5/10000,Trigger)</f>
-        <v>1.2499999999999979E-5</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="90"/>
       <c r="Z5" s="3"/>
@@ -13049,7 +13049,7 @@
       </c>
       <c r="T6" s="102"/>
       <c r="U6" s="199">
-        <v>5</v>
+        <v>4.875</v>
       </c>
       <c r="V6" s="102"/>
       <c r="W6" s="208">
@@ -13057,7 +13057,7 @@
       </c>
       <c r="X6" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/10000,Trigger)</f>
-        <v>-3.749999999999999E-5</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="90"/>
       <c r="Z6" s="3"/>
@@ -13333,7 +13333,7 @@
       </c>
       <c r="T10" s="102"/>
       <c r="U10" s="199">
-        <v>5.875</v>
+        <v>6.125</v>
       </c>
       <c r="V10" s="102"/>
       <c r="W10" s="208">
@@ -13341,7 +13341,7 @@
       </c>
       <c r="X10" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/10000,Trigger)</f>
-        <v>-1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="90"/>
       <c r="Z10" s="3"/>
@@ -13393,14 +13393,14 @@
         <v>AUBR6AB3Y=ICAA</v>
       </c>
       <c r="Q11" s="200">
-        <v>5.625</v>
+        <v>5.75</v>
       </c>
       <c r="R11" s="200">
-        <v>7.625</v>
+        <v>7.75</v>
       </c>
       <c r="S11" s="191">
         <f>_xll.qlMidEquivalent(Q11,R11)</f>
-        <v>6.625</v>
+        <v>6.75</v>
       </c>
       <c r="T11" s="102"/>
       <c r="U11" s="199">
@@ -13408,11 +13408,11 @@
       </c>
       <c r="V11" s="102"/>
       <c r="W11" s="208">
-        <v>6.625</v>
+        <v>6.75</v>
       </c>
       <c r="X11" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/10000,Trigger)</f>
-        <v>-2.4999999999999957E-5</v>
+        <v>1.2500000000000033E-5</v>
       </c>
       <c r="Y11" s="90"/>
       <c r="Z11" s="3"/>
@@ -13464,26 +13464,26 @@
         <v>AUBR6AB4Y=ICAA</v>
       </c>
       <c r="Q12" s="200">
-        <v>6.125</v>
+        <v>6.25</v>
       </c>
       <c r="R12" s="200">
-        <v>8.125</v>
+        <v>8.25</v>
       </c>
       <c r="S12" s="191">
         <f>_xll.qlMidEquivalent(Q12,R12)</f>
-        <v>7.125</v>
+        <v>7.25</v>
       </c>
       <c r="T12" s="102"/>
       <c r="U12" s="199">
-        <v>7.125</v>
+        <v>7.25</v>
       </c>
       <c r="V12" s="102"/>
       <c r="W12" s="208">
-        <v>7.125</v>
+        <v>7.25</v>
       </c>
       <c r="X12" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/10000,Trigger)</f>
-        <v>-1.2499999999999924E-5</v>
+        <v>1.2499999999999924E-5</v>
       </c>
       <c r="Y12" s="90"/>
       <c r="Z12" s="3"/>
@@ -13535,26 +13535,26 @@
         <v>AUBR6AB5Y=ICAA</v>
       </c>
       <c r="Q13" s="200">
-        <v>6.5</v>
+        <v>6.625</v>
       </c>
       <c r="R13" s="200">
-        <v>8.5</v>
+        <v>8.625</v>
       </c>
       <c r="S13" s="191">
         <f>_xll.qlMidEquivalent(Q13,R13)</f>
-        <v>7.5</v>
+        <v>7.625</v>
       </c>
       <c r="T13" s="102"/>
       <c r="U13" s="199">
-        <v>7.375</v>
+        <v>7.625</v>
       </c>
       <c r="V13" s="102"/>
       <c r="W13" s="208">
-        <v>7.5</v>
+        <v>7.625</v>
       </c>
       <c r="X13" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/10000,Trigger)</f>
-        <v>0</v>
+        <v>1.2500000000000033E-5</v>
       </c>
       <c r="Y13" s="90"/>
       <c r="Z13" s="3"/>
@@ -13677,26 +13677,26 @@
         <v>AUBR6AB7Y=ICAA</v>
       </c>
       <c r="Q15" s="200">
-        <v>6.5</v>
+        <v>6.75</v>
       </c>
       <c r="R15" s="200">
-        <v>8.5</v>
+        <v>8.75</v>
       </c>
       <c r="S15" s="191">
         <f>_xll.qlMidEquivalent(Q15,R15)</f>
-        <v>7.5</v>
+        <v>7.75</v>
       </c>
       <c r="T15" s="102"/>
       <c r="U15" s="199">
-        <v>7.5</v>
+        <v>7.75</v>
       </c>
       <c r="V15" s="102"/>
       <c r="W15" s="208">
-        <v>7.5</v>
+        <v>7.75</v>
       </c>
       <c r="X15" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/10000,Trigger)</f>
-        <v>-2.4999999999999957E-5</v>
+        <v>2.4999999999999957E-5</v>
       </c>
       <c r="Y15" s="90"/>
       <c r="Z15" s="3"/>
@@ -13890,26 +13890,26 @@
         <v>AUBR6AB10Y=ICAA</v>
       </c>
       <c r="Q18" s="200">
-        <v>6.5</v>
+        <v>6.75</v>
       </c>
       <c r="R18" s="200">
-        <v>8.5</v>
+        <v>8.75</v>
       </c>
       <c r="S18" s="191">
         <f>_xll.qlMidEquivalent(Q18,R18)</f>
-        <v>7.5</v>
+        <v>7.75</v>
       </c>
       <c r="T18" s="102"/>
       <c r="U18" s="199">
-        <v>7.5</v>
+        <v>7.75</v>
       </c>
       <c r="V18" s="102"/>
       <c r="W18" s="208">
-        <v>7.5</v>
+        <v>7.75</v>
       </c>
       <c r="X18" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F18,W18/10000,Trigger)</f>
-        <v>-1.2500000000000033E-5</v>
+        <v>2.4999999999999957E-5</v>
       </c>
       <c r="Y18" s="90"/>
       <c r="Z18" s="3"/>
@@ -14043,7 +14043,7 @@
       </c>
       <c r="T20" s="102"/>
       <c r="U20" s="199">
-        <v>7</v>
+        <v>7.375</v>
       </c>
       <c r="V20" s="102"/>
       <c r="W20" s="208">
@@ -14051,7 +14051,7 @@
       </c>
       <c r="X20" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F20,W20/10000,Trigger)</f>
-        <v>1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="90"/>
       <c r="Z20" s="3"/>
@@ -14256,7 +14256,7 @@
       </c>
       <c r="T23" s="102"/>
       <c r="U23" s="199">
-        <v>6</v>
+        <v>6.375</v>
       </c>
       <c r="V23" s="102"/>
       <c r="W23" s="208">
@@ -14264,7 +14264,7 @@
       </c>
       <c r="X23" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F23,W23/10000,Trigger)</f>
-        <v>1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="90"/>
       <c r="Z23" s="3"/>
@@ -14611,7 +14611,7 @@
       </c>
       <c r="T28" s="102"/>
       <c r="U28" s="199">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="V28" s="102"/>
       <c r="W28" s="208">
@@ -14966,7 +14966,7 @@
       </c>
       <c r="T33" s="102"/>
       <c r="U33" s="199">
-        <v>3.75</v>
+        <v>3.875</v>
       </c>
       <c r="V33" s="102"/>
       <c r="W33" s="208">
@@ -14974,7 +14974,7 @@
       </c>
       <c r="X33" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F33,W33/10000,Trigger)</f>
-        <v>-1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y33" s="90"/>
       <c r="Z33" s="3"/>
@@ -15321,7 +15321,7 @@
       </c>
       <c r="T38" s="102"/>
       <c r="U38" s="199">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="V38" s="102"/>
       <c r="W38" s="208">
@@ -15854,7 +15854,7 @@
       </c>
       <c r="Q5" s="233" t="str">
         <f>_xll.RData(Q6:Q12,R5:T5,"RTFEED:IDN",,,R6)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="R5" s="233" t="s">
         <v>175</v>
@@ -15930,7 +15930,7 @@
         <v>AUCASH=RBAA</v>
       </c>
       <c r="R6" s="273">
-        <v>41850</v>
+        <v>41858</v>
       </c>
       <c r="S6" s="295">
         <v>2.5</v>
@@ -17365,7 +17365,7 @@
       <c r="L4" s="50"/>
       <c r="M4" s="174" t="str">
         <f>_xll.RData(M5:M58,N4:Q4,"RTFEED:IDN",ReutersRtMode,,N5)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="N4" s="171" t="s">
         <v>130</v>
@@ -17631,7 +17631,7 @@
         <v>2.4950000000000001</v>
       </c>
       <c r="O8" s="101">
-        <v>2.5</v>
+        <v>2.5049999999999999</v>
       </c>
       <c r="P8" s="101">
         <v>0</v>
@@ -17641,19 +17641,19 @@
       </c>
       <c r="R8" s="104">
         <f>_xll.qlMidEquivalent($N8,$O8,$P8,$Q8)</f>
-        <v>2.4975000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="S8" s="102"/>
       <c r="T8" s="103">
-        <v>2.4990000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="U8" s="102"/>
       <c r="V8" s="154">
-        <v>2.4975000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="W8" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E8,V8/100,Trigger)</f>
-        <v>0</v>
+        <v>2.5000000000000716E-5</v>
       </c>
       <c r="X8" s="90"/>
       <c r="Z8"/>
@@ -17694,7 +17694,7 @@
         <v>AUD2MOIS=ICAA</v>
       </c>
       <c r="N9" s="101">
-        <v>2.4900000000000002</v>
+        <v>2.492</v>
       </c>
       <c r="O9" s="101">
         <v>2.5</v>
@@ -17707,19 +17707,19 @@
       </c>
       <c r="R9" s="104">
         <f>_xll.qlMidEquivalent($N9,$O9,$P9,$Q9)</f>
-        <v>2.4950000000000001</v>
+        <v>2.496</v>
       </c>
       <c r="S9" s="102"/>
       <c r="T9" s="103">
-        <v>2.4975000000000001</v>
+        <v>2.496</v>
       </c>
       <c r="U9" s="102"/>
       <c r="V9" s="154">
-        <v>2.4950000000000001</v>
+        <v>2.496</v>
       </c>
       <c r="W9" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E9,V9/100,Trigger)</f>
-        <v>9.9999999999961231E-6</v>
+        <v>9.9999999999995925E-6</v>
       </c>
       <c r="X9" s="90"/>
     </row>
@@ -17759,10 +17759,10 @@
         <v>AUD3MOIS=ICAA</v>
       </c>
       <c r="N10" s="101">
-        <v>2.4870000000000001</v>
+        <v>2.4769999999999999</v>
       </c>
       <c r="O10" s="101">
-        <v>2.4950000000000001</v>
+        <v>2.4849999999999999</v>
       </c>
       <c r="P10" s="101">
         <v>0</v>
@@ -17772,19 +17772,19 @@
       </c>
       <c r="R10" s="104">
         <f>_xll.qlMidEquivalent($N10,$O10,$P10,$Q10)</f>
-        <v>2.4910000000000001</v>
+        <v>2.4809999999999999</v>
       </c>
       <c r="S10" s="102"/>
       <c r="T10" s="103">
-        <v>2.4950000000000001</v>
+        <v>2.4809999999999999</v>
       </c>
       <c r="U10" s="102"/>
       <c r="V10" s="154">
-        <v>2.4910000000000001</v>
+        <v>2.4809999999999999</v>
       </c>
       <c r="W10" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E10,V10/100,Trigger)</f>
-        <v>9.9999999999995925E-6</v>
+        <v>-1.0000000000000286E-4</v>
       </c>
       <c r="X10" s="90"/>
     </row>
@@ -17824,10 +17824,10 @@
         <v>AUD4MOIS=ICAA</v>
       </c>
       <c r="N11" s="101">
-        <v>2.4849999999999999</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="O11" s="101">
-        <v>2.4950000000000001</v>
+        <v>2.48</v>
       </c>
       <c r="P11" s="101">
         <v>0</v>
@@ -17837,19 +17837,19 @@
       </c>
       <c r="R11" s="104">
         <f>_xll.qlMidEquivalent($N11,$O11,$P11,$Q11)</f>
-        <v>2.4900000000000002</v>
+        <v>2.4750000000000001</v>
       </c>
       <c r="S11" s="102"/>
       <c r="T11" s="103">
-        <v>2.4925000000000002</v>
+        <v>2.4750000000000001</v>
       </c>
       <c r="U11" s="102"/>
       <c r="V11" s="154">
-        <v>2.4900000000000002</v>
+        <v>2.4750000000000001</v>
       </c>
       <c r="W11" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E11,V11/100,Trigger)</f>
-        <v>3.999999999999837E-5</v>
+        <v>-1.5000000000000083E-4</v>
       </c>
       <c r="X11" s="90"/>
     </row>
@@ -17889,10 +17889,10 @@
         <v>AUD5MOIS=ICAA</v>
       </c>
       <c r="N12" s="101">
-        <v>2.48</v>
+        <v>2.46</v>
       </c>
       <c r="O12" s="101">
-        <v>2.4900000000000002</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="P12" s="101">
         <v>0</v>
@@ -17902,19 +17902,19 @@
       </c>
       <c r="R12" s="104">
         <f>_xll.qlMidEquivalent($N12,$O12,$P12,$Q12)</f>
-        <v>2.4850000000000003</v>
+        <v>2.4649999999999999</v>
       </c>
       <c r="S12" s="102"/>
       <c r="T12" s="103">
-        <v>2.4925000000000002</v>
+        <v>2.4649999999999999</v>
       </c>
       <c r="U12" s="102"/>
       <c r="V12" s="154">
-        <v>2.4850000000000003</v>
+        <v>2.4649999999999999</v>
       </c>
       <c r="W12" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E12,V12/100,Trigger)</f>
-        <v>2.5000000000004186E-5</v>
+        <v>-2.0000000000000573E-4</v>
       </c>
       <c r="X12" s="90"/>
     </row>
@@ -17954,10 +17954,10 @@
         <v>AUD6MOIS=ICAA</v>
       </c>
       <c r="N13" s="101">
-        <v>2.4750000000000001</v>
+        <v>2.452</v>
       </c>
       <c r="O13" s="101">
-        <v>2.4849999999999999</v>
+        <v>2.4630000000000001</v>
       </c>
       <c r="P13" s="101">
         <v>0</v>
@@ -17967,19 +17967,19 @@
       </c>
       <c r="R13" s="104">
         <f>_xll.qlMidEquivalent($N13,$O13,$P13,$Q13)</f>
-        <v>2.48</v>
+        <v>2.4575</v>
       </c>
       <c r="S13" s="102"/>
       <c r="T13" s="103">
-        <v>2.4910000000000001</v>
+        <v>2.4575</v>
       </c>
       <c r="U13" s="102"/>
       <c r="V13" s="154">
-        <v>2.48</v>
+        <v>2.4575</v>
       </c>
       <c r="W13" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E13,V13/100,Trigger)</f>
-        <v>2.4999999999997247E-5</v>
+        <v>-2.2499999999999951E-4</v>
       </c>
       <c r="X13" s="90"/>
     </row>
@@ -18149,10 +18149,10 @@
         <v>AUD9MOIS=ICAA</v>
       </c>
       <c r="N16" s="101">
-        <v>2.4649999999999999</v>
+        <v>2.4369999999999998</v>
       </c>
       <c r="O16" s="101">
-        <v>2.4750000000000001</v>
+        <v>2.4470000000000001</v>
       </c>
       <c r="P16" s="101">
         <v>0</v>
@@ -18162,19 +18162,19 @@
       </c>
       <c r="R16" s="104">
         <f>_xll.qlMidEquivalent($N16,$O16,$P16,$Q16)</f>
-        <v>2.4699999999999998</v>
+        <v>2.4420000000000002</v>
       </c>
       <c r="S16" s="102"/>
       <c r="T16" s="103">
-        <v>2.4900000000000002</v>
+        <v>2.4420000000000002</v>
       </c>
       <c r="U16" s="102"/>
       <c r="V16" s="154">
-        <v>2.4699999999999998</v>
+        <v>2.4420000000000002</v>
       </c>
       <c r="W16" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E16,V16/100,Trigger)</f>
-        <v>-2.5000000000004186E-5</v>
+        <v>-2.7999999999999553E-4</v>
       </c>
       <c r="X16" s="90"/>
     </row>
@@ -18344,10 +18344,10 @@
         <v>AUD12MOIS=ICAA</v>
       </c>
       <c r="N19" s="101">
-        <v>2.4700000000000002</v>
+        <v>2.4369999999999998</v>
       </c>
       <c r="O19" s="101">
-        <v>2.48</v>
+        <v>2.4449999999999998</v>
       </c>
       <c r="P19" s="101">
         <v>0</v>
@@ -18357,19 +18357,19 @@
       </c>
       <c r="R19" s="104">
         <f>_xll.qlMidEquivalent($N19,$O19,$P19,$Q19)</f>
-        <v>2.4750000000000001</v>
+        <v>2.4409999999999998</v>
       </c>
       <c r="S19" s="102"/>
       <c r="T19" s="103">
-        <v>2.5009999999999999</v>
+        <v>2.4409999999999998</v>
       </c>
       <c r="U19" s="102"/>
       <c r="V19" s="154">
-        <v>2.4750000000000001</v>
+        <v>2.4409999999999998</v>
       </c>
       <c r="W19" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E19,V19/100,Trigger)</f>
-        <v>2.5000000000000716E-5</v>
+        <v>-3.4000000000000349E-4</v>
       </c>
       <c r="X19" s="90"/>
     </row>
@@ -18734,10 +18734,10 @@
         <v>AUD18MOIS=ICAA</v>
       </c>
       <c r="N25" s="101">
-        <v>2.5</v>
+        <v>2.4649999999999999</v>
       </c>
       <c r="O25" s="101">
-        <v>2.5500000000000003</v>
+        <v>2.5150000000000001</v>
       </c>
       <c r="P25" s="101">
         <v>0</v>
@@ -18747,19 +18747,19 @@
       </c>
       <c r="R25" s="104">
         <f>_xll.qlMidEquivalent($N25,$O25,$P25,$Q25)</f>
-        <v>2.5250000000000004</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="S25" s="102"/>
       <c r="T25" s="103">
-        <v>2.5649999999999999</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="U25" s="102"/>
       <c r="V25" s="154">
-        <v>2.5250000000000004</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="W25" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E25,V25/100,Trigger)</f>
-        <v>0</v>
+        <v>-3.5000000000000309E-4</v>
       </c>
       <c r="X25" s="90"/>
     </row>
@@ -19124,10 +19124,10 @@
         <v>AUD2YOIS=ICAA</v>
       </c>
       <c r="N31" s="101">
-        <v>2.5750000000000002</v>
+        <v>2.5500000000000003</v>
       </c>
       <c r="O31" s="101">
-        <v>2.625</v>
+        <v>2.6</v>
       </c>
       <c r="P31" s="101">
         <v>0</v>
@@ -19137,19 +19137,19 @@
       </c>
       <c r="R31" s="104">
         <f>_xll.qlMidEquivalent($N31,$O31,$P31,$Q31)</f>
-        <v>2.6</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="S31" s="102"/>
       <c r="T31" s="103">
-        <v>2.65</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="U31" s="102"/>
       <c r="V31" s="154">
-        <v>2.6</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="W31" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E31,V31/100,Trigger)</f>
-        <v>-4.9999999999997963E-5</v>
+        <v>-2.5000000000000022E-4</v>
       </c>
       <c r="X31" s="90"/>
     </row>
@@ -19384,10 +19384,10 @@
         <v>AUD3YOIS=ICAA</v>
       </c>
       <c r="N35" s="101">
-        <v>2.7600000000000002</v>
+        <v>2.7549999999999999</v>
       </c>
       <c r="O35" s="101">
-        <v>2.81</v>
+        <v>2.8050000000000002</v>
       </c>
       <c r="P35" s="101">
         <v>0</v>
@@ -19397,19 +19397,19 @@
       </c>
       <c r="R35" s="104">
         <f>_xll.qlMidEquivalent($N35,$O35,$P35,$Q35)</f>
-        <v>2.7850000000000001</v>
+        <v>2.7800000000000002</v>
       </c>
       <c r="S35" s="102"/>
       <c r="T35" s="103">
-        <v>2.855</v>
+        <v>2.7800000000000002</v>
       </c>
       <c r="U35" s="102"/>
       <c r="V35" s="154">
-        <v>2.7850000000000001</v>
+        <v>2.7800000000000002</v>
       </c>
       <c r="W35" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E35,V35/100,Trigger)</f>
-        <v>-2.5000000000000022E-4</v>
+        <v>-4.9999999999997963E-5</v>
       </c>
       <c r="X35" s="90"/>
     </row>
@@ -21209,7 +21209,7 @@
       <c r="N4" s="50"/>
       <c r="O4" s="174" t="str">
         <f>_xll.RData(O5:O58,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="P4" s="171" t="s">
         <v>130</v>
@@ -22277,32 +22277,32 @@
         <v>AUD1YMTOIS=ICAA</v>
       </c>
       <c r="P19" s="101">
-        <v>2.4580000000000002</v>
+        <v>2.42</v>
       </c>
       <c r="Q19" s="101">
-        <v>2.508</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="R19" s="101">
         <v>0</v>
       </c>
       <c r="S19" s="101">
-        <v>2.4830000000000001</v>
+        <v>2.4449999999999998</v>
       </c>
       <c r="T19" s="104">
         <f>_xll.qlMidEquivalent($P19,$Q19,$R19,$S19)</f>
-        <v>2.4830000000000001</v>
+        <v>2.4450000000000003</v>
       </c>
       <c r="U19" s="102"/>
       <c r="V19" s="103">
-        <v>2.508</v>
+        <v>2.4450000000000003</v>
       </c>
       <c r="W19" s="102"/>
       <c r="X19" s="154">
-        <v>2.4830000000000001</v>
+        <v>2.4450000000000003</v>
       </c>
       <c r="Y19" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F19,X19/100,Trigger)</f>
-        <v>8.000000000000021E-5</v>
+        <v>-3.7999999999999839E-4</v>
       </c>
       <c r="Z19" s="90"/>
     </row>
@@ -22703,32 +22703,32 @@
         <v>AUD18MMTOIS=ICAA</v>
       </c>
       <c r="P25" s="101">
-        <v>2.4849999999999999</v>
+        <v>2.4449999999999998</v>
       </c>
       <c r="Q25" s="101">
-        <v>2.5350000000000001</v>
+        <v>2.4950000000000001</v>
       </c>
       <c r="R25" s="101">
         <v>0</v>
       </c>
       <c r="S25" s="101">
-        <v>2.5100000000000002</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="T25" s="104">
         <f>_xll.qlMidEquivalent($P25,$Q25,$R25,$S25)</f>
-        <v>2.5099999999999998</v>
+        <v>2.4699999999999998</v>
       </c>
       <c r="U25" s="102"/>
       <c r="V25" s="103">
-        <v>2.5449999999999999</v>
+        <v>2.4699999999999998</v>
       </c>
       <c r="W25" s="102"/>
       <c r="X25" s="154">
-        <v>2.5099999999999998</v>
+        <v>2.4699999999999998</v>
       </c>
       <c r="Y25" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F25,X25/100,Trigger)</f>
-        <v>4.9999999999997963E-5</v>
+        <v>-4.0000000000000105E-4</v>
       </c>
       <c r="Z25" s="90"/>
     </row>
@@ -23129,32 +23129,32 @@
         <v>AUD2YMTOIS=ICAA</v>
       </c>
       <c r="P31" s="101">
-        <v>2.5500000000000003</v>
+        <v>2.5150000000000001</v>
       </c>
       <c r="Q31" s="101">
-        <v>2.6</v>
+        <v>2.5649999999999999</v>
       </c>
       <c r="R31" s="101">
         <v>0</v>
       </c>
       <c r="S31" s="101">
-        <v>2.57</v>
+        <v>2.54</v>
       </c>
       <c r="T31" s="104">
         <f>_xll.qlMidEquivalent($P31,$Q31,$R31,$S31)</f>
-        <v>2.5750000000000002</v>
+        <v>2.54</v>
       </c>
       <c r="U31" s="102"/>
       <c r="V31" s="103">
-        <v>2.62</v>
+        <v>2.54</v>
       </c>
       <c r="W31" s="102"/>
       <c r="X31" s="154">
-        <v>2.5750000000000002</v>
+        <v>2.54</v>
       </c>
       <c r="Y31" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F31,X31/100,Trigger)</f>
-        <v>0</v>
+        <v>-3.5000000000000309E-4</v>
       </c>
       <c r="Z31" s="90"/>
     </row>
@@ -23413,32 +23413,32 @@
         <v>AUD3YMTOIS=ICAA</v>
       </c>
       <c r="P35" s="101">
-        <v>2.6850000000000001</v>
+        <v>2.665</v>
       </c>
       <c r="Q35" s="101">
-        <v>2.7349999999999999</v>
+        <v>2.7149999999999999</v>
       </c>
       <c r="R35" s="101">
         <v>0</v>
       </c>
       <c r="S35" s="101">
-        <v>2.7050000000000001</v>
+        <v>2.69</v>
       </c>
       <c r="T35" s="104">
         <f>_xll.qlMidEquivalent($P35,$Q35,$R35,$S35)</f>
-        <v>2.71</v>
+        <v>2.69</v>
       </c>
       <c r="U35" s="102"/>
       <c r="V35" s="103">
-        <v>2.7749999999999999</v>
+        <v>2.69</v>
       </c>
       <c r="W35" s="102"/>
       <c r="X35" s="154">
-        <v>2.71</v>
+        <v>2.69</v>
       </c>
       <c r="Y35" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F35,X35/100,Trigger)</f>
-        <v>-3.0000000000000165E-4</v>
+        <v>-1.9999999999999879E-4</v>
       </c>
       <c r="Z35" s="90"/>
     </row>
@@ -23697,32 +23697,32 @@
         <v>AUD4YMTOIS=ICAA</v>
       </c>
       <c r="P39" s="101">
-        <v>2.8180000000000001</v>
+        <v>2.8130000000000002</v>
       </c>
       <c r="Q39" s="101">
-        <v>2.8679999999999999</v>
+        <v>2.863</v>
       </c>
       <c r="R39" s="101">
         <v>0</v>
       </c>
       <c r="S39" s="101">
-        <v>2.84</v>
+        <v>2.8380000000000001</v>
       </c>
       <c r="T39" s="104">
         <f>_xll.qlMidEquivalent($P39,$Q39,$R39,$S39)</f>
-        <v>2.843</v>
+        <v>2.8380000000000001</v>
       </c>
       <c r="U39" s="102"/>
       <c r="V39" s="103">
-        <v>2.92</v>
+        <v>2.8380000000000001</v>
       </c>
       <c r="W39" s="102"/>
       <c r="X39" s="154">
-        <v>2.843</v>
+        <v>2.8380000000000001</v>
       </c>
       <c r="Y39" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F39,X39/100,Trigger)</f>
-        <v>-2.2000000000000144E-4</v>
+        <v>-4.9999999999997963E-5</v>
       </c>
       <c r="Z39" s="90"/>
     </row>
@@ -23981,32 +23981,32 @@
         <v>AUD5YMTOIS=ICAA</v>
       </c>
       <c r="P43" s="101">
-        <v>2.948</v>
+        <v>2.9550000000000001</v>
       </c>
       <c r="Q43" s="101">
-        <v>2.9980000000000002</v>
+        <v>3.0049999999999999</v>
       </c>
       <c r="R43" s="101">
         <v>0</v>
       </c>
       <c r="S43" s="101">
-        <v>2.97</v>
+        <v>2.98</v>
       </c>
       <c r="T43" s="104">
         <f>_xll.qlMidEquivalent($P43,$Q43,$R43,$S43)</f>
-        <v>2.9729999999999999</v>
+        <v>2.98</v>
       </c>
       <c r="U43" s="102"/>
       <c r="V43" s="103">
-        <v>3.0780000000000003</v>
+        <v>2.98</v>
       </c>
       <c r="W43" s="102"/>
       <c r="X43" s="154">
-        <v>2.9729999999999999</v>
+        <v>2.98</v>
       </c>
       <c r="Y43" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F43,X43/100,Trigger)</f>
-        <v>-3.699999999999988E-4</v>
+        <v>7.0000000000000617E-5</v>
       </c>
       <c r="Z43" s="90"/>
     </row>
@@ -24052,32 +24052,32 @@
         <v>AUD6YMTOIS=ICAA</v>
       </c>
       <c r="P44" s="101">
-        <v>3.0830000000000002</v>
+        <v>3.093</v>
       </c>
       <c r="Q44" s="101">
-        <v>3.133</v>
+        <v>3.1430000000000002</v>
       </c>
       <c r="R44" s="101">
         <v>0</v>
       </c>
       <c r="S44" s="101">
-        <v>3.105</v>
+        <v>3.1179999999999999</v>
       </c>
       <c r="T44" s="104">
         <f>_xll.qlMidEquivalent($P44,$Q44,$R44,$S44)</f>
-        <v>3.1080000000000001</v>
+        <v>3.1180000000000003</v>
       </c>
       <c r="U44" s="102"/>
       <c r="V44" s="103">
-        <v>3.238</v>
+        <v>3.1180000000000003</v>
       </c>
       <c r="W44" s="102"/>
       <c r="X44" s="154">
-        <v>3.1080000000000001</v>
+        <v>3.1180000000000003</v>
       </c>
       <c r="Y44" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F44,X44/100,Trigger)</f>
-        <v>-5.200000000000031E-4</v>
+        <v>1.0000000000000286E-4</v>
       </c>
       <c r="Z44" s="90"/>
     </row>
@@ -24123,32 +24123,32 @@
         <v>AUD7YMTOIS=ICAA</v>
       </c>
       <c r="P45" s="101">
-        <v>3.218</v>
+        <v>3.2280000000000002</v>
       </c>
       <c r="Q45" s="101">
-        <v>3.2680000000000002</v>
+        <v>3.278</v>
       </c>
       <c r="R45" s="101">
         <v>0</v>
       </c>
       <c r="S45" s="101">
-        <v>3.24</v>
+        <v>3.2530000000000001</v>
       </c>
       <c r="T45" s="104">
         <f>_xll.qlMidEquivalent($P45,$Q45,$R45,$S45)</f>
-        <v>3.2430000000000003</v>
+        <v>3.2530000000000001</v>
       </c>
       <c r="U45" s="102"/>
       <c r="V45" s="103">
-        <v>3.3980000000000001</v>
+        <v>3.2530000000000001</v>
       </c>
       <c r="W45" s="102"/>
       <c r="X45" s="154">
-        <v>3.2430000000000003</v>
+        <v>3.2530000000000001</v>
       </c>
       <c r="Y45" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F45,X45/100,Trigger)</f>
-        <v>-6.499999999999978E-4</v>
+        <v>1.0000000000000286E-4</v>
       </c>
       <c r="Z45" s="90"/>
     </row>
@@ -24194,32 +24194,32 @@
         <v>AUD8YMTOIS=ICAA</v>
       </c>
       <c r="P46" s="101">
-        <v>3.3080000000000003</v>
+        <v>3.3200000000000003</v>
       </c>
       <c r="Q46" s="101">
-        <v>3.3580000000000001</v>
+        <v>3.37</v>
       </c>
       <c r="R46" s="101">
         <v>0</v>
       </c>
       <c r="S46" s="101">
-        <v>3.33</v>
+        <v>3.3450000000000002</v>
       </c>
       <c r="T46" s="104">
         <f>_xll.qlMidEquivalent($P46,$Q46,$R46,$S46)</f>
-        <v>3.3330000000000002</v>
+        <v>3.3450000000000002</v>
       </c>
       <c r="U46" s="102"/>
       <c r="V46" s="103">
-        <v>3.5049999999999999</v>
+        <v>3.3450000000000002</v>
       </c>
       <c r="W46" s="102"/>
       <c r="X46" s="154">
-        <v>3.3330000000000002</v>
+        <v>3.3450000000000002</v>
       </c>
       <c r="Y46" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F46,X46/100,Trigger)</f>
-        <v>-7.5000000000000761E-4</v>
+        <v>1.2000000000000205E-4</v>
       </c>
       <c r="Z46" s="90"/>
     </row>
@@ -24265,32 +24265,32 @@
         <v>AUD9YMTOIS=ICAA</v>
       </c>
       <c r="P47" s="101">
-        <v>3.3980000000000001</v>
+        <v>3.41</v>
       </c>
       <c r="Q47" s="101">
-        <v>3.448</v>
+        <v>3.46</v>
       </c>
       <c r="R47" s="101">
         <v>0</v>
       </c>
       <c r="S47" s="101">
-        <v>3.423</v>
+        <v>3.4350000000000001</v>
       </c>
       <c r="T47" s="104">
         <f>_xll.qlMidEquivalent($P47,$Q47,$R47,$S47)</f>
-        <v>3.423</v>
+        <v>3.4350000000000001</v>
       </c>
       <c r="U47" s="102"/>
       <c r="V47" s="103">
-        <v>3.61</v>
+        <v>3.4350000000000001</v>
       </c>
       <c r="W47" s="102"/>
       <c r="X47" s="154">
-        <v>3.423</v>
+        <v>3.4350000000000001</v>
       </c>
       <c r="Y47" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F47,X47/100,Trigger)</f>
-        <v>-8.4999999999999659E-4</v>
+        <v>1.1999999999999511E-4</v>
       </c>
       <c r="Z47" s="90"/>
     </row>
@@ -24336,32 +24336,32 @@
         <v>AUD10YMTOIS=ICAA</v>
       </c>
       <c r="P48" s="101">
-        <v>3.488</v>
+        <v>3.5030000000000001</v>
       </c>
       <c r="Q48" s="101">
-        <v>3.5380000000000003</v>
+        <v>3.5529999999999999</v>
       </c>
       <c r="R48" s="101">
         <v>0</v>
       </c>
       <c r="S48" s="101">
-        <v>3.5129999999999999</v>
+        <v>3.528</v>
       </c>
       <c r="T48" s="104">
         <f>_xll.qlMidEquivalent($P48,$Q48,$R48,$S48)</f>
-        <v>3.5129999999999999</v>
+        <v>3.528</v>
       </c>
       <c r="U48" s="102"/>
       <c r="V48" s="103">
-        <v>3.718</v>
+        <v>3.528</v>
       </c>
       <c r="W48" s="102"/>
       <c r="X48" s="154">
-        <v>3.5129999999999999</v>
+        <v>3.528</v>
       </c>
       <c r="Y48" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F48,X48/100,Trigger)</f>
-        <v>-9.4999999999999946E-4</v>
+        <v>1.4999999999999736E-4</v>
       </c>
       <c r="Z48" s="90"/>
     </row>
@@ -24407,32 +24407,32 @@
         <v>AUD12YMTOIS=ICAA</v>
       </c>
       <c r="P49" s="101">
-        <v>3.6230000000000002</v>
+        <v>3.64</v>
       </c>
       <c r="Q49" s="101">
-        <v>3.673</v>
+        <v>3.69</v>
       </c>
       <c r="R49" s="101">
         <v>0</v>
       </c>
       <c r="S49" s="101">
-        <v>3.6480000000000001</v>
+        <v>3.665</v>
       </c>
       <c r="T49" s="104">
         <f>_xll.qlMidEquivalent($P49,$Q49,$R49,$S49)</f>
-        <v>3.6480000000000001</v>
+        <v>3.665</v>
       </c>
       <c r="U49" s="102"/>
       <c r="V49" s="103">
-        <v>3.8650000000000002</v>
+        <v>3.665</v>
       </c>
       <c r="W49" s="102"/>
       <c r="X49" s="154">
-        <v>3.6480000000000001</v>
+        <v>3.665</v>
       </c>
       <c r="Y49" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F49,X49/100,Trigger)</f>
-        <v>-1.1000000000000038E-3</v>
+        <v>1.7000000000000348E-4</v>
       </c>
       <c r="Z49" s="90"/>
     </row>
@@ -24478,32 +24478,32 @@
         <v>AUD15YMTOIS=ICAA</v>
       </c>
       <c r="P50" s="101">
-        <v>3.77</v>
+        <v>3.7880000000000003</v>
       </c>
       <c r="Q50" s="101">
-        <v>3.8200000000000003</v>
+        <v>3.8380000000000001</v>
       </c>
       <c r="R50" s="101">
         <v>0</v>
       </c>
       <c r="S50" s="101">
-        <v>3.7949999999999999</v>
+        <v>3.8130000000000002</v>
       </c>
       <c r="T50" s="104">
         <f>_xll.qlMidEquivalent($P50,$Q50,$R50,$S50)</f>
-        <v>3.7949999999999999</v>
+        <v>3.8130000000000002</v>
       </c>
       <c r="U50" s="102"/>
       <c r="V50" s="103">
-        <v>4.008</v>
+        <v>3.8130000000000002</v>
       </c>
       <c r="W50" s="102"/>
       <c r="X50" s="154">
-        <v>3.7949999999999999</v>
+        <v>3.8130000000000002</v>
       </c>
       <c r="Y50" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F50,X50/100,Trigger)</f>
-        <v>-1.130000000000006E-3</v>
+        <v>1.8000000000000654E-4</v>
       </c>
       <c r="Z50" s="90"/>
     </row>
@@ -24549,32 +24549,32 @@
         <v>AUD20YMTOIS=ICAA</v>
       </c>
       <c r="P51" s="101">
-        <v>3.915</v>
+        <v>3.93</v>
       </c>
       <c r="Q51" s="101">
-        <v>3.9650000000000003</v>
+        <v>3.98</v>
       </c>
       <c r="R51" s="101">
         <v>0</v>
       </c>
       <c r="S51" s="101">
-        <v>3.94</v>
+        <v>3.9550000000000001</v>
       </c>
       <c r="T51" s="104">
         <f>_xll.qlMidEquivalent($P51,$Q51,$R51,$S51)</f>
-        <v>3.9400000000000004</v>
+        <v>3.9550000000000001</v>
       </c>
       <c r="U51" s="102"/>
       <c r="V51" s="103">
-        <v>4.1379999999999999</v>
+        <v>3.9550000000000001</v>
       </c>
       <c r="W51" s="102"/>
       <c r="X51" s="154">
-        <v>3.9400000000000004</v>
+        <v>3.9550000000000001</v>
       </c>
       <c r="Y51" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F51,X51/100,Trigger)</f>
-        <v>-9.7999999999999476E-4</v>
+        <v>1.4999999999999736E-4</v>
       </c>
       <c r="Z51" s="90"/>
     </row>
@@ -24620,32 +24620,32 @@
         <v>AUD25YMTOIS=ICAA</v>
       </c>
       <c r="P52" s="101">
-        <v>3.9849999999999999</v>
+        <v>4.0030000000000001</v>
       </c>
       <c r="Q52" s="101">
-        <v>4.0350000000000001</v>
+        <v>4.0529999999999999</v>
       </c>
       <c r="R52" s="101">
         <v>0</v>
       </c>
       <c r="S52" s="101">
-        <v>4.01</v>
+        <v>4.0280000000000005</v>
       </c>
       <c r="T52" s="104">
         <f>_xll.qlMidEquivalent($P52,$Q52,$R52,$S52)</f>
-        <v>4.01</v>
+        <v>4.0280000000000005</v>
       </c>
       <c r="U52" s="102"/>
       <c r="V52" s="103">
-        <v>4.1929999999999996</v>
+        <v>4.0280000000000005</v>
       </c>
       <c r="W52" s="102"/>
       <c r="X52" s="154">
-        <v>4.01</v>
+        <v>4.0280000000000005</v>
       </c>
       <c r="Y52" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F52,X52/100,Trigger)</f>
-        <v>-9.3000000000000027E-4</v>
+        <v>1.8000000000000654E-4</v>
       </c>
       <c r="Z52" s="90"/>
     </row>
@@ -24762,32 +24762,32 @@
         <v>AUD30YMTOIS=ICAA</v>
       </c>
       <c r="P54" s="101">
-        <v>4.0200000000000005</v>
+        <v>4.0380000000000003</v>
       </c>
       <c r="Q54" s="101">
-        <v>4.07</v>
+        <v>4.0880000000000001</v>
       </c>
       <c r="R54" s="101">
         <v>0</v>
       </c>
       <c r="S54" s="101">
-        <v>4.0449999999999999</v>
+        <v>4.0629999999999997</v>
       </c>
       <c r="T54" s="104">
         <f>_xll.qlMidEquivalent($P54,$Q54,$R54,$S54)</f>
-        <v>4.0449999999999999</v>
+        <v>4.0630000000000006</v>
       </c>
       <c r="U54" s="102"/>
       <c r="V54" s="103">
-        <v>4.2149999999999999</v>
+        <v>4.0630000000000006</v>
       </c>
       <c r="W54" s="102"/>
       <c r="X54" s="154">
-        <v>4.0449999999999999</v>
+        <v>4.0630000000000006</v>
       </c>
       <c r="Y54" s="100">
         <f>_xll.qlSimpleQuoteSetValue(F54,X54/100,Trigger)</f>
-        <v>-8.3000000000000435E-4</v>
+        <v>1.8000000000000654E-4</v>
       </c>
       <c r="Z54" s="90"/>
     </row>
@@ -25338,7 +25338,7 @@
       <c r="Q3" s="124"/>
       <c r="R3" s="123">
         <f>_xll.ohTrigger(R5:R18)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S3" s="90"/>
       <c r="T3" s="3"/>
@@ -25368,7 +25368,7 @@
       <c r="I4" s="120"/>
       <c r="J4" s="98" t="str">
         <f>_xll.RData(J6:J22,K4:L4,,ReutersRtMode,,K6)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="K4" s="98" t="s">
         <v>130</v>
@@ -25879,7 +25879,7 @@
       </c>
       <c r="N13" s="102"/>
       <c r="O13" s="103">
-        <v>2.6749999999999998</v>
+        <v>2.6750000000000003</v>
       </c>
       <c r="P13" s="102"/>
       <c r="Q13" s="154">
@@ -26319,7 +26319,7 @@
       </c>
       <c r="N21" s="102"/>
       <c r="O21" s="103">
-        <v>2.9249999999999998</v>
+        <v>2.9250000000000003</v>
       </c>
       <c r="P21" s="102"/>
       <c r="Q21" s="154">
@@ -26665,7 +26665,7 @@
       <c r="M4" s="29"/>
       <c r="N4" s="307" t="str">
         <f>_xll.RData(N5:N19,O4:R4,"RTFEED:IDN",ReutersRtMode,,O5)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="O4" s="121" t="s">
         <v>130</v>
@@ -26739,10 +26739,10 @@
         <v>AUD1X4F=</v>
       </c>
       <c r="O5" s="136">
-        <v>2.62</v>
+        <v>2.58</v>
       </c>
       <c r="P5" s="136">
-        <v>2.65</v>
+        <v>2.61</v>
       </c>
       <c r="Q5" s="105">
         <v>0</v>
@@ -26752,20 +26752,20 @@
       </c>
       <c r="S5" s="313">
         <f>_xll.qlMidSafe($O5,$P5)</f>
-        <v>2.6349999999999998</v>
+        <v>2.5949999999999998</v>
       </c>
       <c r="T5" s="102"/>
       <c r="U5" s="138">
-        <v>2.7</v>
+        <v>2.5949999999999998</v>
       </c>
       <c r="V5" s="102"/>
       <c r="W5" s="161">
         <f t="array" ref="W5:W19">QuoteLive</f>
-        <v>2.6349999999999998</v>
+        <v>2.5949999999999998</v>
       </c>
       <c r="X5" s="113">
         <f>_xll.qlSimpleQuoteSetValue(E5,W5/100,Trigger)</f>
-        <v>-3.0000000000000165E-4</v>
+        <v>-4.0000000000000105E-4</v>
       </c>
       <c r="Y5" s="90"/>
       <c r="Z5" s="3"/>
@@ -26812,10 +26812,10 @@
         <v>AUD2X5F=</v>
       </c>
       <c r="O6" s="136">
-        <v>2.6</v>
+        <v>2.56</v>
       </c>
       <c r="P6" s="136">
-        <v>2.63</v>
+        <v>2.59</v>
       </c>
       <c r="Q6" s="105">
         <v>0</v>
@@ -26825,15 +26825,15 @@
       </c>
       <c r="S6" s="313">
         <f>_xll.qlMidSafe($O6,$P6)</f>
-        <v>2.6150000000000002</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="T6" s="102"/>
       <c r="U6" s="134">
-        <v>2.665</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="V6" s="102"/>
       <c r="W6" s="154">
-        <v>2.6150000000000002</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="X6" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E6,W6/100,Trigger)</f>
@@ -26884,32 +26884,32 @@
         <v>AUD3X6F=</v>
       </c>
       <c r="O7" s="136">
-        <v>2.59</v>
+        <v>2.54</v>
       </c>
       <c r="P7" s="136">
-        <v>2.62</v>
+        <v>2.57</v>
       </c>
       <c r="Q7" s="105">
         <v>0</v>
       </c>
       <c r="R7" s="136">
-        <v>2.59</v>
+        <v>2.6</v>
       </c>
       <c r="S7" s="313">
         <f>_xll.qlMidSafe($O7,$P7)</f>
-        <v>2.605</v>
+        <v>2.5549999999999997</v>
       </c>
       <c r="T7" s="102"/>
       <c r="U7" s="134">
-        <v>2.6550000000000002</v>
+        <v>2.5549999999999997</v>
       </c>
       <c r="V7" s="102"/>
       <c r="W7" s="154">
-        <v>2.605</v>
+        <v>2.5549999999999997</v>
       </c>
       <c r="X7" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E7,W7/100,Trigger)</f>
-        <v>-2.9999999999999818E-4</v>
+        <v>-5.0000000000000391E-4</v>
       </c>
       <c r="Y7" s="90"/>
       <c r="Z7" s="3"/>
@@ -26956,32 +26956,32 @@
         <v>AUD4X7F=</v>
       </c>
       <c r="O8" s="136">
-        <v>2.58</v>
+        <v>2.5300000000000002</v>
       </c>
       <c r="P8" s="136">
-        <v>2.61</v>
+        <v>2.56</v>
       </c>
       <c r="Q8" s="105">
         <v>0</v>
       </c>
       <c r="R8" s="136">
-        <v>2.58</v>
+        <v>2.59</v>
       </c>
       <c r="S8" s="313">
         <f>_xll.qlMidSafe($O8,$P8)</f>
-        <v>2.5949999999999998</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="T8" s="102"/>
       <c r="U8" s="134">
-        <v>2.645</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="V8" s="102"/>
       <c r="W8" s="154">
-        <v>2.5949999999999998</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="X8" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E8,W8/100,Trigger)</f>
-        <v>-2.0000000000000573E-4</v>
+        <v>-4.9999999999999697E-4</v>
       </c>
       <c r="Y8" s="90"/>
       <c r="Z8" s="3"/>
@@ -27028,32 +27028,32 @@
         <v>AUD5X8F=</v>
       </c>
       <c r="O9" s="136">
-        <v>2.57</v>
+        <v>2.5300000000000002</v>
       </c>
       <c r="P9" s="136">
-        <v>2.6</v>
+        <v>2.56</v>
       </c>
       <c r="Q9" s="105">
         <v>0</v>
       </c>
       <c r="R9" s="136">
-        <v>2.58</v>
+        <v>2.6</v>
       </c>
       <c r="S9" s="313">
         <f>_xll.qlMidSafe($O9,$P9)</f>
-        <v>2.585</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="T9" s="102"/>
       <c r="U9" s="134">
-        <v>2.645</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="V9" s="102"/>
       <c r="W9" s="154">
-        <v>2.585</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="X9" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E9,W9/100,Trigger)</f>
-        <v>-2.0000000000000226E-4</v>
+        <v>-3.9999999999999758E-4</v>
       </c>
       <c r="Y9" s="90"/>
       <c r="Z9" s="3"/>
@@ -27100,32 +27100,32 @@
         <v>AUD6X9F=</v>
       </c>
       <c r="O10" s="136">
-        <v>2.57</v>
+        <v>2.5300000000000002</v>
       </c>
       <c r="P10" s="136">
-        <v>2.6</v>
+        <v>2.56</v>
       </c>
       <c r="Q10" s="105">
         <v>0</v>
       </c>
       <c r="R10" s="136">
-        <v>2.58</v>
+        <v>2.6</v>
       </c>
       <c r="S10" s="313">
         <f>_xll.qlMidSafe($O10,$P10)</f>
-        <v>2.585</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="T10" s="102"/>
       <c r="U10" s="134">
-        <v>2.645</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="V10" s="102"/>
       <c r="W10" s="154">
-        <v>2.585</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="X10" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E10,W10/100,Trigger)</f>
-        <v>-2.0000000000000226E-4</v>
+        <v>-3.9999999999999758E-4</v>
       </c>
       <c r="Y10" s="90"/>
       <c r="Z10" s="3"/>
@@ -27190,7 +27190,7 @@
       </c>
       <c r="T11" s="102"/>
       <c r="U11" s="309">
-        <v>2.69</v>
+        <v>2.63</v>
       </c>
       <c r="V11" s="102"/>
       <c r="W11" s="310">
@@ -27198,7 +27198,7 @@
       </c>
       <c r="X11" s="311">
         <f>_xll.qlSimpleQuoteSetValue(E11,W11/100,Trigger)</f>
-        <v>-3.9999999999999758E-4</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="90"/>
       <c r="Z11" s="3"/>
@@ -27246,10 +27246,10 @@
         <v>AUD2X8F=</v>
       </c>
       <c r="O12" s="136">
-        <v>2.6</v>
+        <v>2.61</v>
       </c>
       <c r="P12" s="136">
-        <v>2.64</v>
+        <v>2.65</v>
       </c>
       <c r="Q12" s="105">
         <v>0</v>
@@ -27259,19 +27259,19 @@
       </c>
       <c r="S12" s="313">
         <f>_xll.qlMidSafe($O12,$P12)</f>
-        <v>2.62</v>
+        <v>2.63</v>
       </c>
       <c r="T12" s="102"/>
       <c r="U12" s="134">
-        <v>2.68</v>
+        <v>2.63</v>
       </c>
       <c r="V12" s="102"/>
       <c r="W12" s="154">
-        <v>2.62</v>
+        <v>2.63</v>
       </c>
       <c r="X12" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E12,W12/100,Trigger)</f>
-        <v>-2.9999999999999818E-4</v>
+        <v>9.9999999999999395E-5</v>
       </c>
       <c r="Y12" s="90"/>
       <c r="Z12" s="3"/>
@@ -27319,32 +27319,32 @@
         <v>AUD3X9F=</v>
       </c>
       <c r="O13" s="136">
-        <v>2.59</v>
+        <v>2.61</v>
       </c>
       <c r="P13" s="136">
-        <v>2.63</v>
+        <v>2.65</v>
       </c>
       <c r="Q13" s="105">
         <v>0</v>
       </c>
       <c r="R13" s="136">
-        <v>2.6</v>
+        <v>2.61</v>
       </c>
       <c r="S13" s="313">
         <f>_xll.qlMidSafe($O13,$P13)</f>
-        <v>2.61</v>
+        <v>2.63</v>
       </c>
       <c r="T13" s="102"/>
       <c r="U13" s="134">
-        <v>2.67</v>
+        <v>2.63</v>
       </c>
       <c r="V13" s="102"/>
       <c r="W13" s="154">
-        <v>2.61</v>
+        <v>2.63</v>
       </c>
       <c r="X13" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E13,W13/100,Trigger)</f>
-        <v>-3.0000000000000165E-4</v>
+        <v>2.0000000000000226E-4</v>
       </c>
       <c r="Y13" s="90"/>
       <c r="Z13" s="3"/>
@@ -27392,32 +27392,32 @@
         <v>AUD4X10F=</v>
       </c>
       <c r="O14" s="136">
-        <v>2.59</v>
+        <v>2.61</v>
       </c>
       <c r="P14" s="136">
-        <v>2.63</v>
+        <v>2.65</v>
       </c>
       <c r="Q14" s="105">
         <v>0</v>
       </c>
       <c r="R14" s="136">
-        <v>2.6</v>
+        <v>2.61</v>
       </c>
       <c r="S14" s="313">
         <f>_xll.qlMidSafe($O14,$P14)</f>
-        <v>2.61</v>
+        <v>2.63</v>
       </c>
       <c r="T14" s="102"/>
       <c r="U14" s="134">
-        <v>2.67</v>
+        <v>2.63</v>
       </c>
       <c r="V14" s="102"/>
       <c r="W14" s="154">
-        <v>2.61</v>
+        <v>2.63</v>
       </c>
       <c r="X14" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E14,W14/100,Trigger)</f>
-        <v>-3.0000000000000165E-4</v>
+        <v>2.0000000000000226E-4</v>
       </c>
       <c r="Y14" s="90"/>
       <c r="Z14" s="3"/>
@@ -27465,32 +27465,32 @@
         <v>AUD5X11F=</v>
       </c>
       <c r="O15" s="136">
-        <v>2.59</v>
+        <v>2.62</v>
       </c>
       <c r="P15" s="136">
-        <v>2.63</v>
+        <v>2.66</v>
       </c>
       <c r="Q15" s="105">
         <v>0</v>
       </c>
       <c r="R15" s="136">
-        <v>2.6</v>
+        <v>2.62</v>
       </c>
       <c r="S15" s="313">
         <f>_xll.qlMidSafe($O15,$P15)</f>
-        <v>2.61</v>
+        <v>2.64</v>
       </c>
       <c r="T15" s="102"/>
       <c r="U15" s="134">
-        <v>2.68</v>
+        <v>2.64</v>
       </c>
       <c r="V15" s="102"/>
       <c r="W15" s="154">
-        <v>2.61</v>
+        <v>2.64</v>
       </c>
       <c r="X15" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E15,W15/100,Trigger)</f>
-        <v>-2.0000000000000226E-4</v>
+        <v>3.0000000000000165E-4</v>
       </c>
       <c r="Y15" s="90"/>
       <c r="Z15" s="3"/>
@@ -27538,32 +27538,32 @@
         <v>AUD6X12F=</v>
       </c>
       <c r="O16" s="136">
-        <v>2.6</v>
+        <v>2.63</v>
       </c>
       <c r="P16" s="136">
-        <v>2.64</v>
+        <v>2.67</v>
       </c>
       <c r="Q16" s="105">
         <v>0</v>
       </c>
       <c r="R16" s="136">
-        <v>2.61</v>
+        <v>2.63</v>
       </c>
       <c r="S16" s="313">
         <f>_xll.qlMidSafe($O16,$P16)</f>
-        <v>2.62</v>
+        <v>2.65</v>
       </c>
       <c r="T16" s="102"/>
       <c r="U16" s="134">
-        <v>2.68</v>
+        <v>2.65</v>
       </c>
       <c r="V16" s="102"/>
       <c r="W16" s="154">
-        <v>2.62</v>
+        <v>2.65</v>
       </c>
       <c r="X16" s="100">
         <f>_xll.qlSimpleQuoteSetValue(E16,W16/100,Trigger)</f>
-        <v>-1.9999999999999879E-4</v>
+        <v>2.9999999999999818E-4</v>
       </c>
       <c r="Y16" s="90"/>
       <c r="Z16" s="3"/>
@@ -27968,7 +27968,7 @@
       </c>
       <c r="O2" s="98" t="str">
         <f>_xll.RData(O3:O14,P2:T2,"RTFEED:IDN",ReutersRtMode,,P3)</f>
-        <v>Updated at 11:09:33</v>
+        <v>Updated at 17:59:27</v>
       </c>
       <c r="P2" s="143" t="s">
         <v>150</v>
@@ -29518,7 +29518,7 @@
       <c r="Y3" s="51"/>
       <c r="Z3" s="123">
         <f>_xll.ohTrigger(Z5:Z46)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AA3" s="168"/>
       <c r="AB3" s="3"/>
@@ -29577,7 +29577,7 @@
       </c>
       <c r="O4" s="174" t="str">
         <f>_xll.RData(O5:O46,P4:T4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
-        <v>Updated at 11:09:55</v>
+        <v>Updated at 18:00:06</v>
       </c>
       <c r="P4" s="171" t="s">
         <v>150</v>
@@ -29729,7 +29729,7 @@
       </c>
       <c r="AH5" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG5,IborIndex,AF5,F5,Volatility,MeanReversion,Permanent,AND(ISERROR(Z5),ISERROR(FuturesHWConvAdj!Q5:Q6)),ObjectOverwrite)</f>
-        <v>AUDFUT3MQ4ConvAdj_Quote#0003</v>
+        <v>AUDFUT3MQ4ConvAdj_Quote#0005</v>
       </c>
       <c r="AI5" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH5)</f>
@@ -29781,32 +29781,32 @@
         <v>41893</v>
       </c>
       <c r="Q6" s="101">
-        <v>97.37</v>
+        <v>97.39</v>
       </c>
       <c r="R6" s="101">
-        <v>97.38</v>
+        <v>97.4</v>
       </c>
       <c r="S6" s="101">
-        <v>97.37</v>
+        <v>97.4</v>
       </c>
       <c r="T6" s="101">
-        <v>97.36</v>
+        <v>97.4</v>
       </c>
       <c r="U6" s="104">
         <f>_xll.qlMidSafe($Q6,$R6)</f>
-        <v>97.375</v>
+        <v>97.39500000000001</v>
       </c>
       <c r="V6" s="102"/>
-      <c r="W6" s="160" t="e">
-        <v>#NUM!</v>
+      <c r="W6" s="160">
+        <v>97.39500000000001</v>
       </c>
       <c r="X6" s="102"/>
       <c r="Y6" s="154">
-        <v>97.375</v>
-      </c>
-      <c r="Z6" s="104" t="e">
+        <v>97.39500000000001</v>
+      </c>
+      <c r="Z6" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F6,Y6,Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="9"/>
       <c r="AB6" s="3"/>
@@ -29826,7 +29826,7 @@
       </c>
       <c r="AH6" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG6,IborIndex,AF6,F6,Volatility,MeanReversion,Permanent,AND(ISERROR(Z6),ISERROR(FuturesHWConvAdj!Q6:Q7)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU4ConvAdj_Quote#0003</v>
+        <v>AUDFUT3MU4ConvAdj_Quote#0005</v>
       </c>
       <c r="AI6" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH6)</f>
@@ -29894,8 +29894,8 @@
         <v>#NUM!</v>
       </c>
       <c r="V7" s="102"/>
-      <c r="W7" s="160">
-        <v>97.34</v>
+      <c r="W7" s="160" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X7" s="102"/>
       <c r="Y7" s="154" t="e">
@@ -29923,7 +29923,7 @@
       </c>
       <c r="AH7" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG7,IborIndex,AF7,F7,Volatility,MeanReversion,Permanent,AND(ISERROR(Z7),ISERROR(FuturesHWConvAdj!Q7:Q8)),ObjectOverwrite)</f>
-        <v>AUDFUT3MV4ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MV4ConvAdj_Quote#0005</v>
       </c>
       <c r="AI7" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH7)</f>
@@ -30020,7 +30020,7 @@
       </c>
       <c r="AH8" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG8,IborIndex,AF8,F8,Volatility,MeanReversion,Permanent,AND(ISERROR(Z8),ISERROR(FuturesHWConvAdj!Q8:Q9)),ObjectOverwrite)</f>
-        <v>AUDFUT3MX4ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MX4ConvAdj_Quote#0005</v>
       </c>
       <c r="AI8" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH8)</f>
@@ -30073,32 +30073,32 @@
         <v>41984</v>
       </c>
       <c r="Q9" s="101">
-        <v>97.4</v>
+        <v>97.45</v>
       </c>
       <c r="R9" s="101">
-        <v>97.41</v>
+        <v>97.460000000000008</v>
       </c>
       <c r="S9" s="101">
-        <v>97.4</v>
+        <v>97.45</v>
       </c>
       <c r="T9" s="101">
-        <v>97.4</v>
+        <v>97.45</v>
       </c>
       <c r="U9" s="104">
         <f>_xll.qlMidSafe($Q9,$R9)</f>
-        <v>97.405000000000001</v>
+        <v>97.455000000000013</v>
       </c>
       <c r="V9" s="102"/>
-      <c r="W9" s="155" t="e">
-        <v>#NUM!</v>
+      <c r="W9" s="155">
+        <v>97.455000000000013</v>
       </c>
       <c r="X9" s="102"/>
       <c r="Y9" s="154">
-        <v>97.405000000000001</v>
-      </c>
-      <c r="Z9" s="104" t="e">
+        <v>97.455000000000013</v>
+      </c>
+      <c r="Z9" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F9,Y9,Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AA9" s="9"/>
       <c r="AB9" s="3"/>
@@ -30118,7 +30118,7 @@
       </c>
       <c r="AH9" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG9,IborIndex,AF9,F9,Volatility,MeanReversion,Permanent,AND(ISERROR(Z9),ISERROR(FuturesHWConvAdj!Q9:Q10)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ4ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ4ConvAdj_Quote#0005</v>
       </c>
       <c r="AI9" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH9)</f>
@@ -30186,8 +30186,8 @@
         <v>#NUM!</v>
       </c>
       <c r="V10" s="102"/>
-      <c r="W10" s="155">
-        <v>97.35</v>
+      <c r="W10" s="155" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X10" s="102"/>
       <c r="Y10" s="154" t="e">
@@ -30215,7 +30215,7 @@
       </c>
       <c r="AH10" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG10,IborIndex,AF10,F10,Volatility,MeanReversion,Permanent,AND(ISERROR(Z10),ISERROR(FuturesHWConvAdj!Q10:Q11)),ObjectOverwrite)</f>
-        <v>AUDFUT3MF5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MF5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI10" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH10)</f>
@@ -30312,7 +30312,7 @@
       </c>
       <c r="AH11" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG11,IborIndex,AF11,F11,Volatility,MeanReversion,Permanent,AND(ISERROR(Z11),ISERROR(FuturesHWConvAdj!Q11:Q12)),ObjectOverwrite)</f>
-        <v>AUDFUT3MG5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MG5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI11" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH11)</f>
@@ -30364,32 +30364,32 @@
         <v>42075</v>
       </c>
       <c r="Q12" s="101">
-        <v>97.4</v>
+        <v>97.460000000000008</v>
       </c>
       <c r="R12" s="101">
-        <v>97.41</v>
+        <v>97.47</v>
       </c>
       <c r="S12" s="101">
-        <v>97.4</v>
+        <v>97.47</v>
       </c>
       <c r="T12" s="101">
-        <v>97.4</v>
+        <v>97.45</v>
       </c>
       <c r="U12" s="104">
         <f>_xll.qlMidSafe($Q12,$R12)</f>
-        <v>97.405000000000001</v>
+        <v>97.465000000000003</v>
       </c>
       <c r="V12" s="102"/>
-      <c r="W12" s="155" t="e">
-        <v>#NUM!</v>
+      <c r="W12" s="155">
+        <v>97.465000000000003</v>
       </c>
       <c r="X12" s="102"/>
       <c r="Y12" s="154">
-        <v>97.405000000000001</v>
-      </c>
-      <c r="Z12" s="104" t="e">
+        <v>97.465000000000003</v>
+      </c>
+      <c r="Z12" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F12,Y12,Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AA12" s="9"/>
       <c r="AB12" s="3"/>
@@ -30409,7 +30409,7 @@
       </c>
       <c r="AH12" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG12,IborIndex,AF12,F12,Volatility,MeanReversion,Permanent,AND(ISERROR(Z12),ISERROR(FuturesHWConvAdj!Q12:Q13)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MH5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI12" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH12)</f>
@@ -30477,8 +30477,8 @@
         <v>#NUM!</v>
       </c>
       <c r="V13" s="102"/>
-      <c r="W13" s="155">
-        <v>97.33</v>
+      <c r="W13" s="155" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X13" s="102"/>
       <c r="Y13" s="154" t="e">
@@ -30506,7 +30506,7 @@
       </c>
       <c r="AH13" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG13,IborIndex,AF13,F13,Volatility,MeanReversion,Permanent,AND(ISERROR(Z13),ISERROR(FuturesHWConvAdj!Q13:Q14)),ObjectOverwrite)</f>
-        <v>AUDFUT3MJ5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MJ5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI13" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH13)</f>
@@ -30603,7 +30603,7 @@
       </c>
       <c r="AH14" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG14,IborIndex,AF14,F14,Volatility,MeanReversion,Permanent,AND(ISERROR(Z14),ISERROR(FuturesHWConvAdj!Q14:Q15)),ObjectOverwrite)</f>
-        <v>AUDFUT3MK5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MK5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI14" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH14)</f>
@@ -30655,32 +30655,32 @@
         <v>42166</v>
       </c>
       <c r="Q15" s="101">
-        <v>97.350000000000009</v>
+        <v>97.42</v>
       </c>
       <c r="R15" s="101">
-        <v>97.36</v>
+        <v>97.43</v>
       </c>
       <c r="S15" s="101">
-        <v>97.36</v>
+        <v>97.43</v>
       </c>
       <c r="T15" s="101">
-        <v>97.36</v>
+        <v>97.41</v>
       </c>
       <c r="U15" s="104">
         <f>_xll.qlMidSafe($Q15,$R15)</f>
-        <v>97.355000000000004</v>
+        <v>97.425000000000011</v>
       </c>
       <c r="V15" s="102"/>
-      <c r="W15" s="155" t="e">
-        <v>#NUM!</v>
+      <c r="W15" s="155">
+        <v>97.425000000000011</v>
       </c>
       <c r="X15" s="102"/>
       <c r="Y15" s="154">
-        <v>97.355000000000004</v>
-      </c>
-      <c r="Z15" s="104" t="e">
+        <v>97.425000000000011</v>
+      </c>
+      <c r="Z15" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F15,Y15,Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="9"/>
       <c r="AB15" s="3"/>
@@ -30700,7 +30700,7 @@
       </c>
       <c r="AH15" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG15,IborIndex,AF15,F15,Volatility,MeanReversion,Permanent,AND(ISERROR(Z15),ISERROR(FuturesHWConvAdj!Q15:Q16)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MM5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI15" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH15)</f>
@@ -30768,8 +30768,8 @@
         <v>#NUM!</v>
       </c>
       <c r="V16" s="102"/>
-      <c r="W16" s="155">
-        <v>97.25</v>
+      <c r="W16" s="155" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X16" s="102"/>
       <c r="Y16" s="154" t="e">
@@ -30797,7 +30797,7 @@
       </c>
       <c r="AH16" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG16,IborIndex,AF16,F16,Volatility,MeanReversion,Permanent,AND(ISERROR(Z16),ISERROR(FuturesHWConvAdj!Q16:Q17)),ObjectOverwrite)</f>
-        <v>AUDFUT3MN5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MN5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI16" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH16)</f>
@@ -30849,32 +30849,32 @@
         <v>42257</v>
       </c>
       <c r="Q17" s="101">
-        <v>97.26</v>
+        <v>97.33</v>
       </c>
       <c r="R17" s="101">
-        <v>97.27</v>
+        <v>97.34</v>
       </c>
       <c r="S17" s="101">
-        <v>97.27</v>
+        <v>97.34</v>
       </c>
       <c r="T17" s="101">
-        <v>97.26</v>
+        <v>97.320000000000007</v>
       </c>
       <c r="U17" s="104">
         <f>_xll.qlMidSafe($Q17,$R17)</f>
-        <v>97.265000000000001</v>
+        <v>97.335000000000008</v>
       </c>
       <c r="V17" s="102"/>
       <c r="W17" s="155">
-        <v>97.16</v>
+        <v>97.335000000000008</v>
       </c>
       <c r="X17" s="102"/>
       <c r="Y17" s="154">
-        <v>97.265000000000001</v>
+        <v>97.335000000000008</v>
       </c>
       <c r="Z17" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F17,Y17,Trigger)</f>
-        <v>3.4999999999996589E-2</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="9"/>
       <c r="AB17" s="3"/>
@@ -30894,7 +30894,7 @@
       </c>
       <c r="AH17" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG17,IborIndex,AF17,F17,Volatility,MeanReversion,Permanent,AND(ISERROR(Z17),ISERROR(FuturesHWConvAdj!Q17:Q18)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MU5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI17" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH17)</f>
@@ -30946,32 +30946,32 @@
         <v>42348</v>
       </c>
       <c r="Q18" s="101">
-        <v>97.18</v>
+        <v>97.240000000000009</v>
       </c>
       <c r="R18" s="101">
-        <v>97.19</v>
+        <v>97.25</v>
       </c>
       <c r="S18" s="101">
-        <v>97.19</v>
+        <v>97.240000000000009</v>
       </c>
       <c r="T18" s="101">
-        <v>97.19</v>
+        <v>97.210000000000008</v>
       </c>
       <c r="U18" s="104">
         <f>_xll.qlMidSafe($Q18,$R18)</f>
-        <v>97.185000000000002</v>
+        <v>97.245000000000005</v>
       </c>
       <c r="V18" s="102"/>
       <c r="W18" s="155">
-        <v>97.06</v>
+        <v>97.245000000000005</v>
       </c>
       <c r="X18" s="102"/>
       <c r="Y18" s="154">
-        <v>97.185000000000002</v>
+        <v>97.245000000000005</v>
       </c>
       <c r="Z18" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F18,Y18,Trigger)</f>
-        <v>6.0000000000002274E-2</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="9"/>
       <c r="AB18" s="3"/>
@@ -30991,7 +30991,7 @@
       </c>
       <c r="AH18" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG18,IborIndex,AF18,F18,Volatility,MeanReversion,Permanent,AND(ISERROR(Z18),ISERROR(FuturesHWConvAdj!Q18:Q19)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ5ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ5ConvAdj_Quote#0005</v>
       </c>
       <c r="AI18" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH18)</f>
@@ -31043,32 +31043,32 @@
         <v>42439</v>
       </c>
       <c r="Q19" s="101">
-        <v>97.100000000000009</v>
+        <v>97.14</v>
       </c>
       <c r="R19" s="101">
+        <v>97.15</v>
+      </c>
+      <c r="S19" s="101">
+        <v>97.14</v>
+      </c>
+      <c r="T19" s="101">
         <v>97.11</v>
-      </c>
-      <c r="S19" s="101">
-        <v>97.100000000000009</v>
-      </c>
-      <c r="T19" s="101">
-        <v>97.100000000000009</v>
       </c>
       <c r="U19" s="104">
         <f>_xll.qlMidSafe($Q19,$R19)</f>
-        <v>97.105000000000004</v>
+        <v>97.14500000000001</v>
       </c>
       <c r="V19" s="102"/>
       <c r="W19" s="155">
-        <v>96.954999999999998</v>
+        <v>97.134999999999991</v>
       </c>
       <c r="X19" s="102"/>
       <c r="Y19" s="154">
-        <v>97.105000000000004</v>
+        <v>97.14500000000001</v>
       </c>
       <c r="Z19" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F19,Y19,Trigger)</f>
-        <v>7.9999999999998295E-2</v>
+        <v>0</v>
       </c>
       <c r="AA19" s="9"/>
       <c r="AB19" s="3"/>
@@ -31088,7 +31088,7 @@
       </c>
       <c r="AH19" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG19,IborIndex,AF19,F19,Volatility,MeanReversion,Permanent,AND(ISERROR(Z19),ISERROR(FuturesHWConvAdj!Q19:Q20)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH6ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MH6ConvAdj_Quote#0005</v>
       </c>
       <c r="AI19" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH19)</f>
@@ -31140,32 +31140,32 @@
         <v>42530</v>
       </c>
       <c r="Q20" s="101">
-        <v>97.01</v>
+        <v>97.04</v>
       </c>
       <c r="R20" s="101">
-        <v>97.02</v>
+        <v>97.06</v>
       </c>
       <c r="S20" s="101">
-        <v>97.01</v>
+        <v>97.03</v>
       </c>
       <c r="T20" s="101">
-        <v>97.01</v>
+        <v>97</v>
       </c>
       <c r="U20" s="104">
         <f>_xll.qlMidSafe($Q20,$R20)</f>
-        <v>97.015000000000001</v>
+        <v>97.050000000000011</v>
       </c>
       <c r="V20" s="102"/>
       <c r="W20" s="155">
-        <v>96.85499999999999</v>
+        <v>97.034999999999997</v>
       </c>
       <c r="X20" s="102"/>
       <c r="Y20" s="154">
-        <v>97.015000000000001</v>
+        <v>97.050000000000011</v>
       </c>
       <c r="Z20" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F20,Y20,Trigger)</f>
-        <v>9.0000000000003411E-2</v>
+        <v>0</v>
       </c>
       <c r="AA20" s="9"/>
       <c r="AB20" s="3"/>
@@ -31185,7 +31185,7 @@
       </c>
       <c r="AH20" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG20,IborIndex,AF20,F20,Volatility,MeanReversion,Permanent,AND(ISERROR(Z20),ISERROR(FuturesHWConvAdj!Q20:Q21)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM6ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MM6ConvAdj_Quote#0005</v>
       </c>
       <c r="AI20" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH20)</f>
@@ -31237,32 +31237,32 @@
         <v>42621</v>
       </c>
       <c r="Q21" s="101">
-        <v>96.92</v>
+        <v>96.93</v>
       </c>
       <c r="R21" s="101">
-        <v>96.94</v>
+        <v>96.960000000000008</v>
       </c>
       <c r="S21" s="101">
         <v>0</v>
       </c>
       <c r="T21" s="101">
-        <v>96.94</v>
+        <v>96.88</v>
       </c>
       <c r="U21" s="104">
         <f>_xll.qlMidSafe($Q21,$R21)</f>
-        <v>96.93</v>
+        <v>96.945000000000007</v>
       </c>
       <c r="V21" s="102"/>
-      <c r="W21" s="155" t="e">
-        <v>#NUM!</v>
+      <c r="W21" s="155">
+        <v>96.945000000000007</v>
       </c>
       <c r="X21" s="102"/>
       <c r="Y21" s="154">
-        <v>96.93</v>
+        <v>96.945000000000007</v>
       </c>
       <c r="Z21" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F21,Y21,Trigger)</f>
-        <v>9.9999999999994316E-2</v>
+        <v>0</v>
       </c>
       <c r="AA21" s="9"/>
       <c r="AB21" s="3"/>
@@ -31282,7 +31282,7 @@
       </c>
       <c r="AH21" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG21,IborIndex,AF21,F21,Volatility,MeanReversion,Permanent,AND(ISERROR(Z21),ISERROR(FuturesHWConvAdj!Q21:Q22)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU6ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MU6ConvAdj_Quote#0005</v>
       </c>
       <c r="AI21" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH21)</f>
@@ -31334,32 +31334,32 @@
         <v>42712</v>
       </c>
       <c r="Q22" s="101">
-        <v>96.820000000000007</v>
+        <v>96.83</v>
       </c>
       <c r="R22" s="101">
-        <v>96.86</v>
+        <v>96.87</v>
       </c>
       <c r="S22" s="101">
         <v>0</v>
       </c>
       <c r="T22" s="101">
-        <v>96.91</v>
+        <v>96.8</v>
       </c>
       <c r="U22" s="104">
         <f>_xll.qlMidSafe($Q22,$R22)</f>
-        <v>96.84</v>
+        <v>96.85</v>
       </c>
       <c r="V22" s="102"/>
-      <c r="W22" s="155" t="e">
-        <v>#NUM!</v>
+      <c r="W22" s="155">
+        <v>96.85</v>
       </c>
       <c r="X22" s="102"/>
       <c r="Y22" s="154">
-        <v>96.84</v>
+        <v>96.85</v>
       </c>
       <c r="Z22" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F22,Y22,Trigger)</f>
-        <v>9.9999999999994316E-2</v>
+        <v>0</v>
       </c>
       <c r="AA22" s="9"/>
       <c r="AB22" s="3"/>
@@ -31379,7 +31379,7 @@
       </c>
       <c r="AH22" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG22,IborIndex,AF22,F22,Volatility,MeanReversion,Permanent,AND(ISERROR(Z22),ISERROR(FuturesHWConvAdj!Q22:Q23)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ6ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ6ConvAdj_Quote#0005</v>
       </c>
       <c r="AI22" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH22)</f>
@@ -31434,29 +31434,29 @@
         <v>96.72</v>
       </c>
       <c r="R23" s="101">
-        <v>96.78</v>
+        <v>96.76</v>
       </c>
       <c r="S23" s="101">
         <v>0</v>
       </c>
       <c r="T23" s="101">
-        <v>96.64</v>
+        <v>96.69</v>
       </c>
       <c r="U23" s="104">
         <f>_xll.qlMidSafe($Q23,$R23)</f>
-        <v>96.75</v>
+        <v>96.740000000000009</v>
       </c>
       <c r="V23" s="102"/>
-      <c r="W23" s="155" t="e">
-        <v>#NUM!</v>
+      <c r="W23" s="155">
+        <v>96.735000000000014</v>
       </c>
       <c r="X23" s="102"/>
       <c r="Y23" s="154">
-        <v>96.75</v>
+        <v>96.740000000000009</v>
       </c>
       <c r="Z23" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F23,Y23,Trigger)</f>
-        <v>9.9999999999994316E-2</v>
+        <v>4.9999999999954525E-3</v>
       </c>
       <c r="AA23" s="9"/>
       <c r="AB23" s="3"/>
@@ -31476,7 +31476,7 @@
       </c>
       <c r="AH23" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG23,IborIndex,AF23,F23,Volatility,MeanReversion,Permanent,AND(ISERROR(Z23),ISERROR(FuturesHWConvAdj!Q23:Q24)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH7ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MH7ConvAdj_Quote#0005</v>
       </c>
       <c r="AI23" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH23)</f>
@@ -31531,7 +31531,7 @@
         <v>96.61</v>
       </c>
       <c r="R24" s="101">
-        <v>96.7</v>
+        <v>96.65</v>
       </c>
       <c r="S24" s="101">
         <v>0</v>
@@ -31541,19 +31541,19 @@
       </c>
       <c r="U24" s="104">
         <f>_xll.qlMidSafe($Q24,$R24)</f>
-        <v>96.655000000000001</v>
+        <v>96.63</v>
       </c>
       <c r="V24" s="102"/>
-      <c r="W24" s="155" t="e">
-        <v>#NUM!</v>
+      <c r="W24" s="155">
+        <v>96.63</v>
       </c>
       <c r="X24" s="102"/>
       <c r="Y24" s="154">
-        <v>96.655000000000001</v>
+        <v>96.63</v>
       </c>
       <c r="Z24" s="104">
         <f>_xll.qlSimpleQuoteSetValue(F24,Y24,Trigger)</f>
-        <v>9.4999999999998863E-2</v>
+        <v>0</v>
       </c>
       <c r="AA24" s="9"/>
       <c r="AB24" s="3"/>
@@ -31573,7 +31573,7 @@
       </c>
       <c r="AH24" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG24,IborIndex,AF24,F24,Volatility,MeanReversion,Permanent,AND(ISERROR(Z24),ISERROR(FuturesHWConvAdj!Q24:Q25)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM7ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MM7ConvAdj_Quote#0005</v>
       </c>
       <c r="AI24" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH24)</f>
@@ -31670,7 +31670,7 @@
       </c>
       <c r="AH25" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG25,IborIndex,AF25,F25,Volatility,MeanReversion,Permanent,AND(ISERROR(Z25),ISERROR(FuturesHWConvAdj!Q25:Q26)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU7ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MU7ConvAdj_Quote#0005</v>
       </c>
       <c r="AI25" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH25)</f>
@@ -31767,7 +31767,7 @@
       </c>
       <c r="AH26" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG26,IborIndex,AF26,F26,Volatility,MeanReversion,Permanent,AND(ISERROR(Z26),ISERROR(FuturesHWConvAdj!Q26:Q27)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ7ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ7ConvAdj_Quote#0005</v>
       </c>
       <c r="AI26" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH26)</f>
@@ -31864,7 +31864,7 @@
       </c>
       <c r="AH27" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG27,IborIndex,AF27,F27,Volatility,MeanReversion,Permanent,AND(ISERROR(Z27),ISERROR(FuturesHWConvAdj!Q27:Q28)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH8ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MH8ConvAdj_Quote#0005</v>
       </c>
       <c r="AI27" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH27)</f>
@@ -31961,7 +31961,7 @@
       </c>
       <c r="AH28" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG28,IborIndex,AF28,F28,Volatility,MeanReversion,Permanent,AND(ISERROR(Z28),ISERROR(FuturesHWConvAdj!Q28:Q29)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM8ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MM8ConvAdj_Quote#0005</v>
       </c>
       <c r="AI28" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH28)</f>
@@ -32058,7 +32058,7 @@
       </c>
       <c r="AH29" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG29,IborIndex,AF29,F29,Volatility,MeanReversion,Permanent,AND(ISERROR(Z29),ISERROR(FuturesHWConvAdj!Q29:Q30)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU8ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MU8ConvAdj_Quote#0005</v>
       </c>
       <c r="AI29" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH29)</f>
@@ -32155,7 +32155,7 @@
       </c>
       <c r="AH30" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG30,IborIndex,AF30,F30,Volatility,MeanReversion,Permanent,AND(ISERROR(Z30),ISERROR(FuturesHWConvAdj!Q30:Q31)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ8ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ8ConvAdj_Quote#0005</v>
       </c>
       <c r="AI30" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH30)</f>
@@ -32252,7 +32252,7 @@
       </c>
       <c r="AH31" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG31,IborIndex,AF31,F31,Volatility,MeanReversion,Permanent,AND(ISERROR(Z31),ISERROR(FuturesHWConvAdj!Q31:Q32)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH9ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MH9ConvAdj_Quote#0005</v>
       </c>
       <c r="AI31" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH31)</f>
@@ -32349,7 +32349,7 @@
       </c>
       <c r="AH32" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG32,IborIndex,AF32,F32,Volatility,MeanReversion,Permanent,AND(ISERROR(Z32),ISERROR(FuturesHWConvAdj!Q32:Q33)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM9ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MM9ConvAdj_Quote#0005</v>
       </c>
       <c r="AI32" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH32)</f>
@@ -32446,7 +32446,7 @@
       </c>
       <c r="AH33" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG33,IborIndex,AF33,F33,Volatility,MeanReversion,Permanent,AND(ISERROR(Z33),ISERROR(FuturesHWConvAdj!Q33:Q34)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU9ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MU9ConvAdj_Quote#0005</v>
       </c>
       <c r="AI33" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH33)</f>
@@ -32543,7 +32543,7 @@
       </c>
       <c r="AH34" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG34,IborIndex,AF34,F34,Volatility,MeanReversion,Permanent,AND(ISERROR(Z34),ISERROR(FuturesHWConvAdj!Q34:Q35)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ9ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ9ConvAdj_Quote#0005</v>
       </c>
       <c r="AI34" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH34)</f>
@@ -32640,7 +32640,7 @@
       </c>
       <c r="AH35" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG35,IborIndex,AF35,F35,Volatility,MeanReversion,Permanent,AND(ISERROR(Z35),ISERROR(FuturesHWConvAdj!Q35:Q36)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH0ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MH0ConvAdj_Quote#0005</v>
       </c>
       <c r="AI35" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH35)</f>
@@ -32737,7 +32737,7 @@
       </c>
       <c r="AH36" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG36,IborIndex,AF36,F36,Volatility,MeanReversion,Permanent,AND(ISERROR(Z36),ISERROR(FuturesHWConvAdj!Q36:Q37)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM0ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MM0ConvAdj_Quote#0005</v>
       </c>
       <c r="AI36" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH36)</f>
@@ -32834,7 +32834,7 @@
       </c>
       <c r="AH37" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG37,IborIndex,AF37,F37,Volatility,MeanReversion,Permanent,AND(ISERROR(Z37),ISERROR(FuturesHWConvAdj!Q37:Q38)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU0ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MU0ConvAdj_Quote#0005</v>
       </c>
       <c r="AI37" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH37)</f>
@@ -32931,7 +32931,7 @@
       </c>
       <c r="AH38" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG38,IborIndex,AF38,F38,Volatility,MeanReversion,Permanent,AND(ISERROR(Z38),ISERROR(FuturesHWConvAdj!Q38:Q39)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ0ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ0ConvAdj_Quote#0005</v>
       </c>
       <c r="AI38" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH38)</f>
@@ -33028,7 +33028,7 @@
       </c>
       <c r="AH39" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG39,IborIndex,AF39,F39,Volatility,MeanReversion,Permanent,AND(ISERROR(Z39),ISERROR(FuturesHWConvAdj!Q39:Q40)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH1ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MH1ConvAdj_Quote#0005</v>
       </c>
       <c r="AI39" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH39)</f>
@@ -33125,7 +33125,7 @@
       </c>
       <c r="AH40" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG40,IborIndex,AF40,F40,Volatility,MeanReversion,Permanent,AND(ISERROR(Z40),ISERROR(FuturesHWConvAdj!Q40:Q41)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM1ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MM1ConvAdj_Quote#0005</v>
       </c>
       <c r="AI40" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH40)</f>
@@ -33222,7 +33222,7 @@
       </c>
       <c r="AH41" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG41,IborIndex,AF41,F41,Volatility,MeanReversion,Permanent,AND(ISERROR(Z41),ISERROR(FuturesHWConvAdj!Q41:Q42)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU1ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MU1ConvAdj_Quote#0005</v>
       </c>
       <c r="AI41" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH41)</f>
@@ -33319,7 +33319,7 @@
       </c>
       <c r="AH42" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG42,IborIndex,AF42,F42,Volatility,MeanReversion,Permanent,AND(ISERROR(Z42),ISERROR(FuturesHWConvAdj!Q42:Q43)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ1ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ1ConvAdj_Quote#0005</v>
       </c>
       <c r="AI42" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH42)</f>
@@ -33416,7 +33416,7 @@
       </c>
       <c r="AH43" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG43,IborIndex,AF43,F43,Volatility,MeanReversion,Permanent,AND(ISERROR(Z43),ISERROR(FuturesHWConvAdj!Q43:Q44)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH2ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MH2ConvAdj_Quote#0005</v>
       </c>
       <c r="AI43" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH43)</f>
@@ -33513,7 +33513,7 @@
       </c>
       <c r="AH44" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG44,IborIndex,AF44,F44,Volatility,MeanReversion,Permanent,AND(ISERROR(Z44),ISERROR(FuturesHWConvAdj!Q44:Q45)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM2ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MM2ConvAdj_Quote#0005</v>
       </c>
       <c r="AI44" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH44)</f>
@@ -33610,7 +33610,7 @@
       </c>
       <c r="AH45" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG45,IborIndex,AF45,F45,Volatility,MeanReversion,Permanent,AND(ISERROR(Z45),ISERROR(FuturesHWConvAdj!Q45:Q46)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU2ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MU2ConvAdj_Quote#0005</v>
       </c>
       <c r="AI45" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH45)</f>
@@ -33707,7 +33707,7 @@
       </c>
       <c r="AH46" s="93" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG46,IborIndex,AF46,F46,Volatility,MeanReversion,Permanent,AND(ISERROR(Z46),ISERROR(FuturesHWConvAdj!Q46:Q47)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ2ConvAdj_Quote#0001</v>
+        <v>AUDFUT3MZ2ConvAdj_Quote#0005</v>
       </c>
       <c r="AI46" s="17" t="str">
         <f>_xll.ohRangeRetrieveError(AH46)</f>

</xml_diff>